<commit_message>
Prorate interest when the loan has an early payoff.
The principal change is to the PeriodicInterestBearingWorkingBalance class, which has been extended to include logic for track the last payment date for purposes of calculating the prorated interest.

This change also includes refactoring of the code to calculate loan interest to put the math into a common helper function. Other classes which perform loan interest type calculations all reference this helper code now.
</commit_message>
<xml_diff>
--- a/Retirement SimulatorTests/MonthlyMortgageInterestCalculation.xlsx
+++ b/Retirement SimulatorTests/MonthlyMortgageInterestCalculation.xlsx
@@ -4,84 +4,95 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19560" yWindow="1580" windowWidth="21900" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="2340" windowWidth="24920" windowHeight="16240" tabRatio="823" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Deferred Future Loan UT (5)" sheetId="9" r:id="rId1"/>
-    <sheet name="Deferred Future Loan UT (4)" sheetId="8" r:id="rId2"/>
-    <sheet name="Deferred Future Loan UT (3)" sheetId="7" r:id="rId3"/>
-    <sheet name="Deferred Payment Unit Test" sheetId="6" r:id="rId4"/>
-    <sheet name="Scratchpad for Testing" sheetId="1" r:id="rId5"/>
-    <sheet name="testSimpleLoan unit test" sheetId="3" r:id="rId6"/>
-    <sheet name="testFutureLoan02 unit test" sheetId="2" r:id="rId7"/>
-    <sheet name="Deferred Future Loan UT (2)" sheetId="5" r:id="rId8"/>
-    <sheet name="Deferred Future Loan UT" sheetId="4" r:id="rId9"/>
+    <sheet name="Scratchpad for Testing" sheetId="1" r:id="rId1"/>
+    <sheet name="Early Payoff" sheetId="10" r:id="rId2"/>
+    <sheet name="Deferred Future Loan UT (5)" sheetId="9" r:id="rId3"/>
+    <sheet name="Deferred Future Loan UT (4)" sheetId="8" r:id="rId4"/>
+    <sheet name="Deferred Future Loan UT (3)" sheetId="7" r:id="rId5"/>
+    <sheet name="Deferred Payment Unit Test" sheetId="6" r:id="rId6"/>
+    <sheet name="testSimpleLoan unit test" sheetId="3" r:id="rId7"/>
+    <sheet name="testFutureLoan02 unit test" sheetId="2" r:id="rId8"/>
+    <sheet name="Deferred Future Loan UT (2)" sheetId="5" r:id="rId9"/>
+    <sheet name="Deferred Future Loan UT" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="DeferMonths" localSheetId="7">'Deferred Future Loan UT (2)'!$F$5</definedName>
-    <definedName name="DeferMonths" localSheetId="2">'Deferred Future Loan UT (3)'!$F$5</definedName>
-    <definedName name="DeferMonths" localSheetId="1">'Deferred Future Loan UT (4)'!$F$5</definedName>
-    <definedName name="DeferMonths" localSheetId="0">'Deferred Future Loan UT (5)'!$F$5</definedName>
+    <definedName name="AdjustedAnnualRate">'Early Payoff'!$B$8</definedName>
+    <definedName name="AjustedAnnualRate">'Early Payoff'!$B$8</definedName>
+    <definedName name="DailyRate">'Early Payoff'!$B$9</definedName>
+    <definedName name="DeferMonths" localSheetId="8">'Deferred Future Loan UT (2)'!$F$5</definedName>
+    <definedName name="DeferMonths" localSheetId="4">'Deferred Future Loan UT (3)'!$F$5</definedName>
+    <definedName name="DeferMonths" localSheetId="3">'Deferred Future Loan UT (4)'!$F$5</definedName>
+    <definedName name="DeferMonths" localSheetId="2">'Deferred Future Loan UT (5)'!$F$5</definedName>
     <definedName name="DeferMonths">'Deferred Future Loan UT'!$F$5</definedName>
-    <definedName name="InterestRate" localSheetId="8">'Deferred Future Loan UT'!$B$4</definedName>
-    <definedName name="InterestRate" localSheetId="7">'Deferred Future Loan UT (2)'!$B$4</definedName>
-    <definedName name="InterestRate" localSheetId="2">'Deferred Future Loan UT (3)'!$B$4</definedName>
-    <definedName name="InterestRate" localSheetId="1">'Deferred Future Loan UT (4)'!$B$4</definedName>
-    <definedName name="InterestRate" localSheetId="0">'Deferred Future Loan UT (5)'!$B$4</definedName>
-    <definedName name="InterestRate" localSheetId="3">'Deferred Payment Unit Test'!$B$4</definedName>
-    <definedName name="InterestRate" localSheetId="6">'testFutureLoan02 unit test'!$B$2</definedName>
-    <definedName name="InterestRate" localSheetId="5">'testSimpleLoan unit test'!$B$2</definedName>
+    <definedName name="InterestRate" localSheetId="9">'Deferred Future Loan UT'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="8">'Deferred Future Loan UT (2)'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="4">'Deferred Future Loan UT (3)'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="3">'Deferred Future Loan UT (4)'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="2">'Deferred Future Loan UT (5)'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="5">'Deferred Payment Unit Test'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="1">'Early Payoff'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="7">'testFutureLoan02 unit test'!$B$2</definedName>
+    <definedName name="InterestRate" localSheetId="6">'testSimpleLoan unit test'!$B$2</definedName>
     <definedName name="InterestRate">'Scratchpad for Testing'!$B$2</definedName>
-    <definedName name="Loan_Amount" localSheetId="8">'Deferred Future Loan UT'!$A$3</definedName>
-    <definedName name="Loan_Amount" localSheetId="7">'Deferred Future Loan UT (2)'!$A$3</definedName>
-    <definedName name="Loan_Amount" localSheetId="2">'Deferred Future Loan UT (3)'!$A$3</definedName>
-    <definedName name="Loan_Amount" localSheetId="1">'Deferred Future Loan UT (4)'!$A$3</definedName>
-    <definedName name="Loan_Amount" localSheetId="0">'Deferred Future Loan UT (5)'!$A$3</definedName>
-    <definedName name="Loan_Amount" localSheetId="3">'Deferred Payment Unit Test'!$A$3</definedName>
-    <definedName name="Loan_Amount" localSheetId="6">'testFutureLoan02 unit test'!$A$1</definedName>
-    <definedName name="Loan_Amount" localSheetId="5">'testSimpleLoan unit test'!$A$1</definedName>
+    <definedName name="Loan_Amount" localSheetId="9">'Deferred Future Loan UT'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="8">'Deferred Future Loan UT (2)'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="4">'Deferred Future Loan UT (3)'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="3">'Deferred Future Loan UT (4)'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="2">'Deferred Future Loan UT (5)'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="5">'Deferred Payment Unit Test'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="1">'Early Payoff'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="7">'testFutureLoan02 unit test'!$A$1</definedName>
+    <definedName name="Loan_Amount" localSheetId="6">'testSimpleLoan unit test'!$A$1</definedName>
     <definedName name="Loan_Amount">'Scratchpad for Testing'!$A$1</definedName>
-    <definedName name="LoanAmount" localSheetId="8">'Deferred Future Loan UT'!$B$3</definedName>
-    <definedName name="LoanAmount" localSheetId="7">'Deferred Future Loan UT (2)'!$B$3</definedName>
-    <definedName name="LoanAmount" localSheetId="2">'Deferred Future Loan UT (3)'!$B$3</definedName>
-    <definedName name="LoanAmount" localSheetId="1">'Deferred Future Loan UT (4)'!$B$3</definedName>
-    <definedName name="LoanAmount" localSheetId="0">'Deferred Future Loan UT (5)'!$B$3</definedName>
-    <definedName name="LoanAmount" localSheetId="3">'Deferred Payment Unit Test'!$B$3</definedName>
-    <definedName name="LoanAmount" localSheetId="6">'testFutureLoan02 unit test'!$B$1</definedName>
-    <definedName name="LoanAmount" localSheetId="5">'testSimpleLoan unit test'!$B$1</definedName>
+    <definedName name="LoanAmount" localSheetId="9">'Deferred Future Loan UT'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="8">'Deferred Future Loan UT (2)'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="4">'Deferred Future Loan UT (3)'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="3">'Deferred Future Loan UT (4)'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="2">'Deferred Future Loan UT (5)'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="5">'Deferred Payment Unit Test'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="1">'Early Payoff'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="7">'testFutureLoan02 unit test'!$B$1</definedName>
+    <definedName name="LoanAmount" localSheetId="6">'testSimpleLoan unit test'!$B$1</definedName>
     <definedName name="LoanAmount">'Scratchpad for Testing'!$B$1</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="8">'Deferred Future Loan UT'!$B$5</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="7">'Deferred Future Loan UT (2)'!$B$5</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="2">'Deferred Future Loan UT (3)'!$B$5</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="1">'Deferred Future Loan UT (4)'!$B$5</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="0">'Deferred Future Loan UT (5)'!$B$5</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="3">'Deferred Payment Unit Test'!$B$5</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="6">'testFutureLoan02 unit test'!$B$3</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="5">'testSimpleLoan unit test'!$B$3</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="9">'Deferred Future Loan UT'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="8">'Deferred Future Loan UT (2)'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="4">'Deferred Future Loan UT (3)'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="3">'Deferred Future Loan UT (4)'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="2">'Deferred Future Loan UT (5)'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="5">'Deferred Payment Unit Test'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="1">'Early Payoff'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="7">'testFutureLoan02 unit test'!$B$3</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="6">'testSimpleLoan unit test'!$B$3</definedName>
     <definedName name="MonthlyInterestRate">'Scratchpad for Testing'!$B$3</definedName>
-    <definedName name="MonthlyMultiplier" localSheetId="7">'Deferred Future Loan UT (2)'!$F$3</definedName>
-    <definedName name="MonthlyMultiplier" localSheetId="2">'Deferred Future Loan UT (3)'!$F$3</definedName>
-    <definedName name="MonthlyMultiplier" localSheetId="1">'Deferred Future Loan UT (4)'!$F$3</definedName>
-    <definedName name="MonthlyMultiplier" localSheetId="0">'Deferred Future Loan UT (5)'!$F$3</definedName>
+    <definedName name="MonthlyMultiplier" localSheetId="8">'Deferred Future Loan UT (2)'!$F$3</definedName>
+    <definedName name="MonthlyMultiplier" localSheetId="4">'Deferred Future Loan UT (3)'!$F$3</definedName>
+    <definedName name="MonthlyMultiplier" localSheetId="3">'Deferred Future Loan UT (4)'!$F$3</definedName>
+    <definedName name="MonthlyMultiplier" localSheetId="2">'Deferred Future Loan UT (5)'!$F$3</definedName>
     <definedName name="MonthlyMultiplier">'Deferred Future Loan UT'!$F$3</definedName>
-    <definedName name="MonthlyPayment" localSheetId="8">'Deferred Future Loan UT'!$B$7</definedName>
-    <definedName name="MonthlyPayment" localSheetId="7">'Deferred Future Loan UT (2)'!$B$7</definedName>
-    <definedName name="MonthlyPayment" localSheetId="2">'Deferred Future Loan UT (3)'!$B$7</definedName>
-    <definedName name="MonthlyPayment" localSheetId="1">'Deferred Future Loan UT (4)'!$B$7</definedName>
-    <definedName name="MonthlyPayment" localSheetId="0">'Deferred Future Loan UT (5)'!$B$7</definedName>
-    <definedName name="MonthlyPayment" localSheetId="3">'Deferred Payment Unit Test'!$B$7</definedName>
-    <definedName name="MonthlyPayment" localSheetId="6">'testFutureLoan02 unit test'!$B$5</definedName>
-    <definedName name="MonthlyPayment" localSheetId="5">'testSimpleLoan unit test'!$B$5</definedName>
+    <definedName name="MonthlyPayment" localSheetId="9">'Deferred Future Loan UT'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="8">'Deferred Future Loan UT (2)'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="4">'Deferred Future Loan UT (3)'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="3">'Deferred Future Loan UT (4)'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="2">'Deferred Future Loan UT (5)'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="5">'Deferred Payment Unit Test'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="1">'Early Payoff'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="7">'testFutureLoan02 unit test'!$B$5</definedName>
+    <definedName name="MonthlyPayment" localSheetId="6">'testSimpleLoan unit test'!$B$5</definedName>
     <definedName name="MonthlyPayment">'Scratchpad for Testing'!$B$5</definedName>
-    <definedName name="NumPayments" localSheetId="8">'Deferred Future Loan UT'!$B$6</definedName>
-    <definedName name="NumPayments" localSheetId="7">'Deferred Future Loan UT (2)'!$B$6</definedName>
-    <definedName name="NumPayments" localSheetId="2">'Deferred Future Loan UT (3)'!$B$6</definedName>
-    <definedName name="NumPayments" localSheetId="1">'Deferred Future Loan UT (4)'!$B$6</definedName>
-    <definedName name="NumPayments" localSheetId="0">'Deferred Future Loan UT (5)'!$B$6</definedName>
-    <definedName name="NumPayments" localSheetId="3">'Deferred Payment Unit Test'!$B$6</definedName>
-    <definedName name="NumPayments" localSheetId="6">'testFutureLoan02 unit test'!$B$4</definedName>
-    <definedName name="NumPayments" localSheetId="5">'testSimpleLoan unit test'!$B$4</definedName>
+    <definedName name="NumPayments" localSheetId="9">'Deferred Future Loan UT'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="8">'Deferred Future Loan UT (2)'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="4">'Deferred Future Loan UT (3)'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="3">'Deferred Future Loan UT (4)'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="2">'Deferred Future Loan UT (5)'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="5">'Deferred Payment Unit Test'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="1">'Early Payoff'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="7">'testFutureLoan02 unit test'!$B$4</definedName>
+    <definedName name="NumPayments" localSheetId="6">'testSimpleLoan unit test'!$B$4</definedName>
     <definedName name="NumPayments">'Scratchpad for Testing'!$B$4</definedName>
+    <definedName name="ProratedDays">'Early Payoff'!$B$11</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -93,6 +104,64 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Steve Roehling</author>
+  </authors>
+  <commentList>
+    <comment ref="G40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Roehling:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Balance after payoff on 1/1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G45" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Roehling:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The 25.06 is the prorated interest, all except the last day.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Steve Roehling</author>
@@ -126,7 +195,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Steve Roehling</author>
@@ -185,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="58">
   <si>
     <t>Interest Rate</t>
   </si>
@@ -330,6 +399,36 @@
   <si>
     <t>testPastLoanWithDeferredPaymentAndNoPaymentOfInterestWhileInDeferrmentStartPmtsInPastFinishAfterSimStartAndStartingBalance</t>
   </si>
+  <si>
+    <t>End of 2012</t>
+  </si>
+  <si>
+    <t>Starting Cash Bal</t>
+  </si>
+  <si>
+    <t>Daily Interest Rate</t>
+  </si>
+  <si>
+    <t>Adjusted Annual Rate</t>
+  </si>
+  <si>
+    <t>Prorated Days</t>
+  </si>
+  <si>
+    <t>Multiplier for Prorated Interest</t>
+  </si>
+  <si>
+    <t>Prorated Interest</t>
+  </si>
+  <si>
+    <t>From 12/15/2014 to 1/01/2015 (=17 days)</t>
+  </si>
+  <si>
+    <t>testLoanWithEarlyPayoffAndProratedInterest,testLoanWithEarlyPayoffAndProratedInterestEndOfMonth</t>
+  </si>
+  <si>
+    <t>Prorated Balance For Payoff (on 1/1/2014)</t>
+  </si>
 </sst>
 </file>
 
@@ -340,9 +439,9 @@
     <numFmt numFmtId="164" formatCode="0.0000%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -370,6 +469,14 @@
       <color indexed="81"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -401,11 +508,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -420,15 +528,19 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -758,10 +870,2292 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <f>B2/12</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <f>-PMT(MonthlyInterestRate,NumPayments,LoanAmount,0,0)</f>
+        <v>32.267187193837486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
+        <f>B1</f>
+        <v>1000</v>
+      </c>
+      <c r="C8" s="3">
+        <f>(B8*B$3)</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" ref="D8:D24" si="0">MonthlyPayment-C8</f>
+        <v>23.933853860504151</v>
+      </c>
+      <c r="E8" s="3">
+        <f>B8-D8</f>
+        <v>976.0661461394958</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <f>E8</f>
+        <v>976.0661461394958</v>
+      </c>
+      <c r="C9" s="3">
+        <f>(B9*B$3)</f>
+        <v>8.1338845511624651</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>24.133302642675019</v>
+      </c>
+      <c r="E9" s="3">
+        <f>B9-D9</f>
+        <v>951.93284349682074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" ref="B10:B24" si="1">E9</f>
+        <v>951.93284349682074</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ref="C10:C24" si="2">(B10*B$3)</f>
+        <v>7.9327736958068398</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>24.334413498030646</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" ref="E10:E24" si="3">B10-D10</f>
+        <v>927.59842999879004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="1"/>
+        <v>927.59842999879004</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="2"/>
+        <v>7.7299869166565838</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>24.537200277180901</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="3"/>
+        <v>903.06122972160915</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="1"/>
+        <v>903.06122972160915</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="2"/>
+        <v>7.5255102476800761</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>24.741676946157412</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="3"/>
+        <v>878.31955277545171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="1"/>
+        <v>878.31955277545171</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="2"/>
+        <v>7.3193296064620972</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>24.947857587375388</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="3"/>
+        <v>853.37169518807627</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="1"/>
+        <v>853.37169518807627</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>7.1114307932339687</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>25.155756400603519</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="3"/>
+        <v>828.21593878747274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="1"/>
+        <v>828.21593878747274</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="2"/>
+        <v>6.9017994898956063</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>25.365387703941881</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>802.85055108353083</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="1"/>
+        <v>802.85055108353083</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="2"/>
+        <v>6.6904212590294234</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>25.576765934808062</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="3"/>
+        <v>777.27378514872282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="1"/>
+        <v>777.27378514872282</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="2"/>
+        <v>6.4772815429060238</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>25.789905650931463</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="3"/>
+        <v>751.48387949779135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="1"/>
+        <v>751.48387949779135</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="2"/>
+        <v>6.2623656624815949</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>26.004821531355891</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="3"/>
+        <v>725.47905796643545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="1"/>
+        <v>725.47905796643545</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="2"/>
+        <v>6.045658816386962</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>26.221528377450525</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="3"/>
+        <v>699.25752958898488</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="1"/>
+        <v>699.25752958898488</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="2"/>
+        <v>5.8271460799082071</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>26.440041113929279</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="3"/>
+        <v>672.8174884750556</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="1"/>
+        <v>672.8174884750556</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="2"/>
+        <v>5.6068124039587968</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>26.660374789878688</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="3"/>
+        <v>646.15711368517691</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="1"/>
+        <v>646.15711368517691</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="2"/>
+        <v>5.3846426140431412</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>26.882544579794345</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="3"/>
+        <v>619.27456910538251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="1"/>
+        <v>619.27456910538251</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="2"/>
+        <v>5.1606214092115206</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>27.106565784625964</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="3"/>
+        <v>592.1680033207565</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="1"/>
+        <v>592.1680033207565</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
+        <v>4.9347333610063044</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>27.332453832831181</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="3"/>
+        <v>564.83554948792528</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D35" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>F6</f>
+        <v>1095.5832073797985</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <f>(1+MonthlyInterestRate)</f>
+        <v>1.0083333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <f>B4/12</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <f>POWER(F3,DeferMonths)*F4</f>
+        <v>1095.5832073797985</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <f>-PMT(MonthlyInterestRate,NumPayments,LoanAmount,0,0)</f>
+        <v>35.351388438948831</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B3</f>
+        <v>1095.5832073797985</v>
+      </c>
+      <c r="C10" s="3">
+        <f>(B10*B$5)</f>
+        <v>9.1298600614983201</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ref="D10:D26" si="0">MonthlyPayment-C10</f>
+        <v>26.221528377450511</v>
+      </c>
+      <c r="E10" s="3">
+        <f>B10-D10</f>
+        <v>1069.361679002348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3">
+        <f>E10</f>
+        <v>1069.361679002348</v>
+      </c>
+      <c r="C11" s="3">
+        <f>(B11*B$5)</f>
+        <v>8.9113473250195661</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>26.440041113929265</v>
+      </c>
+      <c r="E11" s="3">
+        <f>B11-D11</f>
+        <v>1042.9216378884187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" ref="B12:B26" si="1">E11</f>
+        <v>1042.9216378884187</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ref="C12:C26" si="2">(B12*B$5)</f>
+        <v>8.6910136490701557</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>26.660374789878674</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ref="E12:E26" si="3">B12-D12</f>
+        <v>1016.26126309854</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="1"/>
+        <v>1016.26126309854</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="2"/>
+        <v>8.4688438591545001</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>26.882544579794331</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="3"/>
+        <v>989.3787185187457</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="1"/>
+        <v>989.3787185187457</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>8.2448226543228813</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>27.10656578462595</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="3"/>
+        <v>962.2721527341198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="1"/>
+        <v>962.2721527341198</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="2"/>
+        <v>8.0189346061176643</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>27.332453832831167</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="3"/>
+        <v>934.93969890128858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="1"/>
+        <v>934.93969890128858</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="2"/>
+        <v>7.791164157510738</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>27.560224281438092</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="3"/>
+        <v>907.3794746198505</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="1"/>
+        <v>907.3794746198505</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="2"/>
+        <v>7.561495621832087</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>27.789892817116744</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="3"/>
+        <v>879.58958180273373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="1"/>
+        <v>879.58958180273373</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="2"/>
+        <v>7.3299131816894478</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>28.021475257259382</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="3"/>
+        <v>851.56810654547439</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="1"/>
+        <v>851.56810654547439</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="2"/>
+        <v>7.0964008878789535</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>28.254987551069878</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="3"/>
+        <v>823.31311899440448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="1"/>
+        <v>823.31311899440448</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="2"/>
+        <v>6.8609426582867039</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>28.490445780662128</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="3"/>
+        <v>794.82267321374229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="1"/>
+        <v>794.82267321374229</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="2"/>
+        <v>6.6235222767811859</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>28.727866162167643</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="3"/>
+        <v>766.09480705157466</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>13</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="1"/>
+        <v>766.09480705157466</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="2"/>
+        <v>6.3841233920964555</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>28.967265046852376</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="3"/>
+        <v>737.12754200472227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>14</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="1"/>
+        <v>737.12754200472227</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="2"/>
+        <v>6.1427295167060185</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>29.208658922242812</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="3"/>
+        <v>707.91888308247951</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="1"/>
+        <v>707.91888308247951</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
+        <v>5.8993240256873296</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>29.452064413261503</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="3"/>
+        <v>678.46681866921801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>16</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="1"/>
+        <v>678.46681866921801</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="2"/>
+        <v>5.6538901555768168</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>29.697498283372013</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="3"/>
+        <v>648.76932038584596</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="1"/>
+        <v>648.76932038584596</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="2"/>
+        <v>5.4064110032153829</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>29.944977435733449</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="3"/>
+        <v>618.82434295011251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" ref="B27:B40" si="4">E26</f>
+        <v>618.82434295011251</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" ref="C27:C40" si="5">(B27*B$5)</f>
+        <v>5.1568695245842706</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" ref="D27:D40" si="6">MonthlyPayment-C27</f>
+        <v>30.194518914364561</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" ref="E27:E40" si="7">B27-D27</f>
+        <v>588.6298240357479</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="4"/>
+        <v>588.6298240357479</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="5"/>
+        <v>4.9052485336312328</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="6"/>
+        <v>30.446139905317597</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="7"/>
+        <v>558.18368413043027</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="4"/>
+        <v>558.18368413043027</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="5"/>
+        <v>4.6515307010869185</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="6"/>
+        <v>30.699857737861912</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="7"/>
+        <v>527.4838263925684</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="4"/>
+        <v>527.4838263925684</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="5"/>
+        <v>4.3956985532714032</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="6"/>
+        <v>30.95568988567743</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="7"/>
+        <v>496.52813650689097</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="4"/>
+        <v>496.52813650689097</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="5"/>
+        <v>4.1377344708907584</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="6"/>
+        <v>31.213653968058072</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="7"/>
+        <v>465.31448253883292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>23</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="4"/>
+        <v>465.31448253883292</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="5"/>
+        <v>3.8776206878236077</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="6"/>
+        <v>31.473767751125223</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="7"/>
+        <v>433.84071478770773</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>24</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="4"/>
+        <v>433.84071478770773</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="5"/>
+        <v>3.6153392898975643</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="6"/>
+        <v>31.736049149051269</v>
+      </c>
+      <c r="E33" s="8">
+        <f t="shared" si="7"/>
+        <v>402.10466563865646</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="4"/>
+        <v>402.10466563865646</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="5"/>
+        <v>3.3508722136554705</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="6"/>
+        <v>32.00051622529336</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="7"/>
+        <v>370.10414941336307</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>26</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="4"/>
+        <v>370.10414941336307</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="5"/>
+        <v>3.084201245111359</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="6"/>
+        <v>32.267187193837472</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="7"/>
+        <v>337.83696221952562</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>27</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="4"/>
+        <v>337.83696221952562</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="5"/>
+        <v>2.8153080184960468</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="6"/>
+        <v>32.536080420452784</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="7"/>
+        <v>305.30088179907284</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>28</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="4"/>
+        <v>305.30088179907284</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="5"/>
+        <v>2.5441740149922736</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="6"/>
+        <v>32.807214423956559</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="7"/>
+        <v>272.49366737511627</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>29</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="4"/>
+        <v>272.49366737511627</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="5"/>
+        <v>2.2707805614593024</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="6"/>
+        <v>33.080607877489527</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="7"/>
+        <v>239.41305949762676</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>30</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="4"/>
+        <v>239.41305949762676</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="5"/>
+        <v>1.9951088291468897</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="6"/>
+        <v>33.356279609801945</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="7"/>
+        <v>206.0567798878248</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>31</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="4"/>
+        <v>206.0567798878248</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="5"/>
+        <v>1.7171398323985401</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="6"/>
+        <v>33.634248606550294</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="7"/>
+        <v>172.4225312812745</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>32</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" ref="B41:B45" si="8">E40</f>
+        <v>172.4225312812745</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" ref="C41:C45" si="9">(B41*B$5)</f>
+        <v>1.4368544273439541</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" ref="D41:D45" si="10">MonthlyPayment-C41</f>
+        <v>33.914534011604879</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" ref="E41:E45" si="11">B41-D41</f>
+        <v>138.50799726966963</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>33</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" si="8"/>
+        <v>138.50799726966963</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="9"/>
+        <v>1.1542333105805802</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="10"/>
+        <v>34.197155128368252</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="11"/>
+        <v>104.31084214130138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>34</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" si="8"/>
+        <v>104.31084214130138</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="9"/>
+        <v>0.86925701784417819</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="10"/>
+        <v>34.482131421104654</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="11"/>
+        <v>69.828710720196725</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>35</v>
+      </c>
+      <c r="B44" s="3">
+        <f t="shared" si="8"/>
+        <v>69.828710720196725</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="9"/>
+        <v>0.58190592266830599</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="10"/>
+        <v>34.769482516280526</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="11"/>
+        <v>35.059228203916199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>36</v>
+      </c>
+      <c r="B45" s="3">
+        <f t="shared" si="8"/>
+        <v>35.059228203916199</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="9"/>
+        <v>0.292160235032635</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="10"/>
+        <v>35.059228203916199</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <f>B4/12</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <f>-PMT(MonthlyInterestRate,NumPayments,LoanAmount,0,0)</f>
+        <v>332.14309812851195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="22">
+        <f>POWER(1+B5,12)-1</f>
+        <v>0.12682503013196977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="23">
+        <f>POWER(AdjustedAnnualRate + 1,1/365) - 1</f>
+        <v>3.2718767925188352E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="23"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="23">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="23">
+        <f>POWER(DailyRate+1,ProratedDays)</f>
+        <v>1.0055767734340098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1">
+        <f>E39*B12</f>
+        <v>4052.6131862949933</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="23">
+        <f>B13-E39</f>
+        <v>22.475166643385819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="23"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3">
+        <f>B3</f>
+        <v>10000</v>
+      </c>
+      <c r="C17" s="3">
+        <f>(B17*B$5)</f>
+        <v>100</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ref="D17:D33" si="0">MonthlyPayment-C17</f>
+        <v>232.14309812851195</v>
+      </c>
+      <c r="E17" s="3">
+        <f>B17-D17</f>
+        <v>9767.8569018714879</v>
+      </c>
+      <c r="F17" s="21">
+        <v>40954</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3">
+        <f>E17</f>
+        <v>9767.8569018714879</v>
+      </c>
+      <c r="C18" s="3">
+        <f>(B18*B$5)</f>
+        <v>97.678569018714882</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>234.46452910979707</v>
+      </c>
+      <c r="E18" s="3">
+        <f>B18-D18</f>
+        <v>9533.3923727616911</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" ref="B19:B33" si="1">E18</f>
+        <v>9533.3923727616911</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" ref="C19:C33" si="2">(B19*B$5)</f>
+        <v>95.33392372761692</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>236.80917440089502</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" ref="E19:E33" si="3">B19-D19</f>
+        <v>9296.5831983607968</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="1"/>
+        <v>9296.5831983607968</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="2"/>
+        <v>92.96583198360797</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>239.17726614490397</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="3"/>
+        <v>9057.4059322158937</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="1"/>
+        <v>9057.4059322158937</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="2"/>
+        <v>90.574059322158945</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>241.56903880635301</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="3"/>
+        <v>8815.8368934095415</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="1"/>
+        <v>8815.8368934095415</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="2"/>
+        <v>88.158368934095421</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>243.98472919441653</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="3"/>
+        <v>8571.8521642151245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="1"/>
+        <v>8571.8521642151245</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="2"/>
+        <v>85.718521642151245</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>246.42457648636071</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="3"/>
+        <v>8325.4275877287637</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="1"/>
+        <v>8325.4275877287637</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
+        <v>83.25427587728764</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>248.88882225122433</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="3"/>
+        <v>8076.5387654775395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="1"/>
+        <v>8076.5387654775395</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="2"/>
+        <v>80.765387654775395</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>251.37771047373656</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="3"/>
+        <v>7825.1610550038031</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="1"/>
+        <v>7825.1610550038031</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="2"/>
+        <v>78.251610550038038</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>253.89148757847391</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="3"/>
+        <v>7571.2695674253291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="1"/>
+        <v>7571.2695674253291</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="2"/>
+        <v>75.712695674253297</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>256.43040245425868</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" si="3"/>
+        <v>7314.8391649710702</v>
+      </c>
+      <c r="F27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="8">
+        <f>B2+B3-SUM(C17:D27)</f>
+        <v>16346.425920586367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="1"/>
+        <v>7314.8391649710702</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="2"/>
+        <v>73.148391649710703</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>258.99470647880128</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="3"/>
+        <v>7055.844458492269</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>13</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="1"/>
+        <v>7055.844458492269</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="2"/>
+        <v>70.558444584922697</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>261.58465354358924</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="3"/>
+        <v>6794.2598049486796</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="1"/>
+        <v>6794.2598049486796</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="2"/>
+        <v>67.942598049486804</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>264.20050007902512</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="3"/>
+        <v>6530.0593048696546</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>15</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="1"/>
+        <v>6530.0593048696546</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="2"/>
+        <v>65.300593048696541</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>266.8425050798154</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="3"/>
+        <v>6263.2167997898396</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>16</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="1"/>
+        <v>6263.2167997898396</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="2"/>
+        <v>62.632167997898399</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>269.51093013061353</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="3"/>
+        <v>5993.7058696592258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>17</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="1"/>
+        <v>5993.7058696592258</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="2"/>
+        <v>59.93705869659226</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>272.20603943191969</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="3"/>
+        <v>5721.4998302273061</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>18</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" ref="B34:B47" si="4">E33</f>
+        <v>5721.4998302273061</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" ref="C34:C47" si="5">(B34*B$5)</f>
+        <v>57.214998302273059</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" ref="D34:D47" si="6">MonthlyPayment-C34</f>
+        <v>274.92809982623891</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" ref="E34:E47" si="7">B34-D34</f>
+        <v>5446.5717304010668</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>19</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="4"/>
+        <v>5446.5717304010668</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="5"/>
+        <v>54.465717304010667</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="6"/>
+        <v>277.67738082450126</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="7"/>
+        <v>5168.8943495765652</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>20</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="4"/>
+        <v>5168.8943495765652</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="5"/>
+        <v>51.688943495765656</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="6"/>
+        <v>280.45415463274628</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="7"/>
+        <v>4888.4401949438188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>21</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="4"/>
+        <v>4888.4401949438188</v>
+      </c>
+      <c r="C37" s="3">
+        <f t="shared" si="5"/>
+        <v>48.884401949438193</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="6"/>
+        <v>283.25869617907375</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="7"/>
+        <v>4605.1814987647449</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>22</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="4"/>
+        <v>4605.1814987647449</v>
+      </c>
+      <c r="C38" s="3">
+        <f t="shared" si="5"/>
+        <v>46.051814987647447</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="6"/>
+        <v>286.0912831408645</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="7"/>
+        <v>4319.0902156238808</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>23</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="4"/>
+        <v>4319.0902156238808</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="5"/>
+        <v>43.190902156238806</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="6"/>
+        <v>288.95219597227316</v>
+      </c>
+      <c r="E39" s="8">
+        <f t="shared" si="7"/>
+        <v>4030.1380196516075</v>
+      </c>
+      <c r="F39" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="8">
+        <f>B2+B3-SUM(C17:D39)</f>
+        <v>12360.708743044226</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>24</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="4"/>
+        <v>4030.1380196516075</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" si="5"/>
+        <v>40.301380196516078</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="6"/>
+        <v>291.84171793199584</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="7"/>
+        <v>3738.2963017196116</v>
+      </c>
+      <c r="G40" s="8">
+        <f>G39-E39-B14</f>
+        <v>8308.0955567492329</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>25</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" si="4"/>
+        <v>3738.2963017196116</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="5"/>
+        <v>37.382963017196118</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="6"/>
+        <v>294.76013511131583</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="7"/>
+        <v>3443.5361666082958</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>26</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" si="4"/>
+        <v>3443.5361666082958</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="5"/>
+        <v>34.435361666082962</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="6"/>
+        <v>297.70773646242901</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="7"/>
+        <v>3145.8284301458671</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>27</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" si="4"/>
+        <v>3145.8284301458671</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="5"/>
+        <v>31.458284301458672</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="6"/>
+        <v>300.68481382705329</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="7"/>
+        <v>2845.1436163188137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>28</v>
+      </c>
+      <c r="B44" s="3">
+        <f t="shared" si="4"/>
+        <v>2845.1436163188137</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="5"/>
+        <v>28.451436163188138</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="6"/>
+        <v>303.69166196532382</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="7"/>
+        <v>2541.4519543534898</v>
+      </c>
+      <c r="F44" s="21">
+        <v>41790</v>
+      </c>
+      <c r="G44" s="3">
+        <f>B2+B3-SUM(C17:D44)</f>
+        <v>10699.993252401666</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>29</v>
+      </c>
+      <c r="B45" s="3">
+        <f t="shared" si="4"/>
+        <v>2541.4519543534898</v>
+      </c>
+      <c r="C45" s="3">
+        <f t="shared" si="5"/>
+        <v>25.414519543534897</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="6"/>
+        <v>306.72857858497707</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="7"/>
+        <v>2234.7233757685126</v>
+      </c>
+      <c r="G45" s="3">
+        <f>G44-E44-25.06</f>
+        <v>8133.4812980481756</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" s="3">
+        <f t="shared" si="4"/>
+        <v>2234.7233757685126</v>
+      </c>
+      <c r="C46" s="3">
+        <f t="shared" si="5"/>
+        <v>22.347233757685128</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="6"/>
+        <v>309.79586437082685</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="7"/>
+        <v>1924.9275113976857</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>31</v>
+      </c>
+      <c r="B47" s="3">
+        <f t="shared" si="4"/>
+        <v>1924.9275113976857</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" si="5"/>
+        <v>19.249275113976857</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="6"/>
+        <v>312.89382301453509</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="7"/>
+        <v>1612.0336883831505</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>32</v>
+      </c>
+      <c r="B48" s="3">
+        <f t="shared" ref="B48:B49" si="8">E47</f>
+        <v>1612.0336883831505</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" ref="C48:C49" si="9">(B48*B$5)</f>
+        <v>16.120336883831506</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" ref="D48:D49" si="10">MonthlyPayment-C48</f>
+        <v>316.02276124468045</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" ref="E48:E49" si="11">B48-D48</f>
+        <v>1296.0109271384702</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>33</v>
+      </c>
+      <c r="B49" s="3">
+        <f t="shared" si="8"/>
+        <v>1296.0109271384702</v>
+      </c>
+      <c r="C49" s="3">
+        <f t="shared" si="9"/>
+        <v>12.960109271384702</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="10"/>
+        <v>319.18298885712727</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="11"/>
+        <v>976.82793828134288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>34</v>
+      </c>
+      <c r="B50" s="3">
+        <f t="shared" ref="B50:B52" si="12">E49</f>
+        <v>976.82793828134288</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" ref="C50:C52" si="13">(B50*B$5)</f>
+        <v>9.7682793828134287</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" ref="D50:D52" si="14">MonthlyPayment-C50</f>
+        <v>322.37481874569852</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" ref="E50:E52" si="15">B50-D50</f>
+        <v>654.45311953564442</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>35</v>
+      </c>
+      <c r="B51" s="3">
+        <f t="shared" si="12"/>
+        <v>654.45311953564442</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="13"/>
+        <v>6.544531195356444</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="14"/>
+        <v>325.5985669331555</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="15"/>
+        <v>328.85455260248892</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>36</v>
+      </c>
+      <c r="B52" s="3">
+        <f t="shared" si="12"/>
+        <v>328.85455260248892</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="13"/>
+        <v>3.2885455260248895</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="14"/>
+        <v>328.85455260248705</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="15"/>
+        <v>1.8758328224066645E-12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -1716,7 +4110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
@@ -2655,7 +5049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
@@ -3535,7 +5929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
@@ -4015,457 +6409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4">
-        <f>B2/12</f>
-        <v>8.3333333333333332E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
-        <f>-PMT(MonthlyInterestRate,NumPayments,LoanAmount,0,0)</f>
-        <v>32.267187193837486</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3">
-        <f>B1</f>
-        <v>1000</v>
-      </c>
-      <c r="C8" s="3">
-        <f>(B8*B$3)</f>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" ref="D8:D24" si="0">MonthlyPayment-C8</f>
-        <v>23.933853860504151</v>
-      </c>
-      <c r="E8" s="3">
-        <f>B8-D8</f>
-        <v>976.0661461394958</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" s="3">
-        <f>E8</f>
-        <v>976.0661461394958</v>
-      </c>
-      <c r="C9" s="3">
-        <f>(B9*B$3)</f>
-        <v>8.1338845511624651</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>24.133302642675019</v>
-      </c>
-      <c r="E9" s="3">
-        <f>B9-D9</f>
-        <v>951.93284349682074</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3">
-        <f t="shared" ref="B10:B24" si="1">E9</f>
-        <v>951.93284349682074</v>
-      </c>
-      <c r="C10" s="3">
-        <f t="shared" ref="C10:C24" si="2">(B10*B$3)</f>
-        <v>7.9327736958068398</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>24.334413498030646</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" ref="E10:E24" si="3">B10-D10</f>
-        <v>927.59842999879004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="1"/>
-        <v>927.59842999879004</v>
-      </c>
-      <c r="C11" s="3">
-        <f t="shared" si="2"/>
-        <v>7.7299869166565838</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>24.537200277180901</v>
-      </c>
-      <c r="E11" s="3">
-        <f t="shared" si="3"/>
-        <v>903.06122972160915</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" si="1"/>
-        <v>903.06122972160915</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="shared" si="2"/>
-        <v>7.5255102476800761</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>24.741676946157412</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="3"/>
-        <v>878.31955277545171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="1"/>
-        <v>878.31955277545171</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" si="2"/>
-        <v>7.3193296064620972</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>24.947857587375388</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="3"/>
-        <v>853.37169518807627</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="1"/>
-        <v>853.37169518807627</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" si="2"/>
-        <v>7.1114307932339687</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>25.155756400603519</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="3"/>
-        <v>828.21593878747274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="1"/>
-        <v>828.21593878747274</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="2"/>
-        <v>6.9017994898956063</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>25.365387703941881</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>802.85055108353083</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>9</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="1"/>
-        <v>802.85055108353083</v>
-      </c>
-      <c r="C16" s="3">
-        <f t="shared" si="2"/>
-        <v>6.6904212590294234</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>25.576765934808062</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="3"/>
-        <v>777.27378514872282</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>10</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" si="1"/>
-        <v>777.27378514872282</v>
-      </c>
-      <c r="C17" s="3">
-        <f t="shared" si="2"/>
-        <v>6.4772815429060238</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" si="0"/>
-        <v>25.789905650931463</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="3"/>
-        <v>751.48387949779135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>11</v>
-      </c>
-      <c r="B18" s="3">
-        <f t="shared" si="1"/>
-        <v>751.48387949779135</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="2"/>
-        <v>6.2623656624815949</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
-        <v>26.004821531355891</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="3"/>
-        <v>725.47905796643545</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>12</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" si="1"/>
-        <v>725.47905796643545</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" si="2"/>
-        <v>6.045658816386962</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="0"/>
-        <v>26.221528377450525</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" si="3"/>
-        <v>699.25752958898488</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
-        <v>13</v>
-      </c>
-      <c r="B20" s="3">
-        <f t="shared" si="1"/>
-        <v>699.25752958898488</v>
-      </c>
-      <c r="C20" s="3">
-        <f t="shared" si="2"/>
-        <v>5.8271460799082071</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="0"/>
-        <v>26.440041113929279</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="3"/>
-        <v>672.8174884750556</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" si="1"/>
-        <v>672.8174884750556</v>
-      </c>
-      <c r="C21" s="3">
-        <f t="shared" si="2"/>
-        <v>5.6068124039587968</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>26.660374789878688</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="3"/>
-        <v>646.15711368517691</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
-        <v>15</v>
-      </c>
-      <c r="B22" s="3">
-        <f t="shared" si="1"/>
-        <v>646.15711368517691</v>
-      </c>
-      <c r="C22" s="3">
-        <f t="shared" si="2"/>
-        <v>5.3846426140431412</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="0"/>
-        <v>26.882544579794345</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="3"/>
-        <v>619.27456910538251</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <v>16</v>
-      </c>
-      <c r="B23" s="3">
-        <f t="shared" si="1"/>
-        <v>619.27456910538251</v>
-      </c>
-      <c r="C23" s="3">
-        <f t="shared" si="2"/>
-        <v>5.1606214092115206</v>
-      </c>
-      <c r="D23" s="3">
-        <f t="shared" si="0"/>
-        <v>27.106565784625964</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="3"/>
-        <v>592.1680033207565</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
-        <v>17</v>
-      </c>
-      <c r="B24" s="3">
-        <f t="shared" si="1"/>
-        <v>592.1680033207565</v>
-      </c>
-      <c r="C24" s="3">
-        <f t="shared" si="2"/>
-        <v>4.9347333610063044</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="0"/>
-        <v>27.332453832831181</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="3"/>
-        <v>564.83554948792528</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D35" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
@@ -4915,7 +6859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
@@ -6393,7 +8337,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
@@ -7324,883 +9268,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f>F6</f>
-        <v>1095.5832073797985</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4">
-        <f>(1+MonthlyInterestRate)</f>
-        <v>1.0083333333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4">
-        <f>B4/12</f>
-        <v>8.3333333333333332E-3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <f>POWER(F3,DeferMonths)*F4</f>
-        <v>1095.5832073797985</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <f>-PMT(MonthlyInterestRate,NumPayments,LoanAmount,0,0)</f>
-        <v>35.351388438948831</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3">
-        <f>B3</f>
-        <v>1095.5832073797985</v>
-      </c>
-      <c r="C10" s="3">
-        <f>(B10*B$5)</f>
-        <v>9.1298600614983201</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" ref="D10:D26" si="0">MonthlyPayment-C10</f>
-        <v>26.221528377450511</v>
-      </c>
-      <c r="E10" s="3">
-        <f>B10-D10</f>
-        <v>1069.361679002348</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3">
-        <f>E10</f>
-        <v>1069.361679002348</v>
-      </c>
-      <c r="C11" s="3">
-        <f>(B11*B$5)</f>
-        <v>8.9113473250195661</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>26.440041113929265</v>
-      </c>
-      <c r="E11" s="3">
-        <f>B11-D11</f>
-        <v>1042.9216378884187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" ref="B12:B26" si="1">E11</f>
-        <v>1042.9216378884187</v>
-      </c>
-      <c r="C12" s="3">
-        <f t="shared" ref="C12:C26" si="2">(B12*B$5)</f>
-        <v>8.6910136490701557</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>26.660374789878674</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" ref="E12:E26" si="3">B12-D12</f>
-        <v>1016.26126309854</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="1"/>
-        <v>1016.26126309854</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" si="2"/>
-        <v>8.4688438591545001</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>26.882544579794331</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="3"/>
-        <v>989.3787185187457</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="1"/>
-        <v>989.3787185187457</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" si="2"/>
-        <v>8.2448226543228813</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>27.10656578462595</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="3"/>
-        <v>962.2721527341198</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="1"/>
-        <v>962.2721527341198</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="2"/>
-        <v>8.0189346061176643</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>27.332453832831167</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>934.93969890128858</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="1"/>
-        <v>934.93969890128858</v>
-      </c>
-      <c r="C16" s="3">
-        <f t="shared" si="2"/>
-        <v>7.791164157510738</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>27.560224281438092</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="3"/>
-        <v>907.3794746198505</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17" s="3">
-        <f t="shared" si="1"/>
-        <v>907.3794746198505</v>
-      </c>
-      <c r="C17" s="3">
-        <f t="shared" si="2"/>
-        <v>7.561495621832087</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" si="0"/>
-        <v>27.789892817116744</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" si="3"/>
-        <v>879.58958180273373</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
-        <v>9</v>
-      </c>
-      <c r="B18" s="3">
-        <f t="shared" si="1"/>
-        <v>879.58958180273373</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" si="2"/>
-        <v>7.3299131816894478</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
-        <v>28.021475257259382</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="3"/>
-        <v>851.56810654547439</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>10</v>
-      </c>
-      <c r="B19" s="3">
-        <f t="shared" si="1"/>
-        <v>851.56810654547439</v>
-      </c>
-      <c r="C19" s="3">
-        <f t="shared" si="2"/>
-        <v>7.0964008878789535</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="0"/>
-        <v>28.254987551069878</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" si="3"/>
-        <v>823.31311899440448</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>11</v>
-      </c>
-      <c r="B20" s="3">
-        <f t="shared" si="1"/>
-        <v>823.31311899440448</v>
-      </c>
-      <c r="C20" s="3">
-        <f t="shared" si="2"/>
-        <v>6.8609426582867039</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="0"/>
-        <v>28.490445780662128</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="3"/>
-        <v>794.82267321374229</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>12</v>
-      </c>
-      <c r="B21" s="3">
-        <f t="shared" si="1"/>
-        <v>794.82267321374229</v>
-      </c>
-      <c r="C21" s="3">
-        <f t="shared" si="2"/>
-        <v>6.6235222767811859</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>28.727866162167643</v>
-      </c>
-      <c r="E21" s="8">
-        <f t="shared" si="3"/>
-        <v>766.09480705157466</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
-        <v>13</v>
-      </c>
-      <c r="B22" s="3">
-        <f t="shared" si="1"/>
-        <v>766.09480705157466</v>
-      </c>
-      <c r="C22" s="3">
-        <f t="shared" si="2"/>
-        <v>6.3841233920964555</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="0"/>
-        <v>28.967265046852376</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="3"/>
-        <v>737.12754200472227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>14</v>
-      </c>
-      <c r="B23" s="3">
-        <f t="shared" si="1"/>
-        <v>737.12754200472227</v>
-      </c>
-      <c r="C23" s="3">
-        <f t="shared" si="2"/>
-        <v>6.1427295167060185</v>
-      </c>
-      <c r="D23" s="3">
-        <f t="shared" si="0"/>
-        <v>29.208658922242812</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="3"/>
-        <v>707.91888308247951</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
-        <v>15</v>
-      </c>
-      <c r="B24" s="3">
-        <f t="shared" si="1"/>
-        <v>707.91888308247951</v>
-      </c>
-      <c r="C24" s="3">
-        <f t="shared" si="2"/>
-        <v>5.8993240256873296</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="0"/>
-        <v>29.452064413261503</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="3"/>
-        <v>678.46681866921801</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25">
-        <v>16</v>
-      </c>
-      <c r="B25" s="3">
-        <f t="shared" si="1"/>
-        <v>678.46681866921801</v>
-      </c>
-      <c r="C25" s="3">
-        <f t="shared" si="2"/>
-        <v>5.6538901555768168</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="0"/>
-        <v>29.697498283372013</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="shared" si="3"/>
-        <v>648.76932038584596</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26">
-        <v>17</v>
-      </c>
-      <c r="B26" s="3">
-        <f t="shared" si="1"/>
-        <v>648.76932038584596</v>
-      </c>
-      <c r="C26" s="3">
-        <f t="shared" si="2"/>
-        <v>5.4064110032153829</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="0"/>
-        <v>29.944977435733449</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="3"/>
-        <v>618.82434295011251</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27">
-        <v>18</v>
-      </c>
-      <c r="B27" s="3">
-        <f t="shared" ref="B27:B40" si="4">E26</f>
-        <v>618.82434295011251</v>
-      </c>
-      <c r="C27" s="3">
-        <f t="shared" ref="C27:C40" si="5">(B27*B$5)</f>
-        <v>5.1568695245842706</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" ref="D27:D40" si="6">MonthlyPayment-C27</f>
-        <v>30.194518914364561</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" ref="E27:E40" si="7">B27-D27</f>
-        <v>588.6298240357479</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28">
-        <v>19</v>
-      </c>
-      <c r="B28" s="3">
-        <f t="shared" si="4"/>
-        <v>588.6298240357479</v>
-      </c>
-      <c r="C28" s="3">
-        <f t="shared" si="5"/>
-        <v>4.9052485336312328</v>
-      </c>
-      <c r="D28" s="3">
-        <f t="shared" si="6"/>
-        <v>30.446139905317597</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="shared" si="7"/>
-        <v>558.18368413043027</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29">
-        <v>20</v>
-      </c>
-      <c r="B29" s="3">
-        <f t="shared" si="4"/>
-        <v>558.18368413043027</v>
-      </c>
-      <c r="C29" s="3">
-        <f t="shared" si="5"/>
-        <v>4.6515307010869185</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="6"/>
-        <v>30.699857737861912</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="shared" si="7"/>
-        <v>527.4838263925684</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30">
-        <v>21</v>
-      </c>
-      <c r="B30" s="3">
-        <f t="shared" si="4"/>
-        <v>527.4838263925684</v>
-      </c>
-      <c r="C30" s="3">
-        <f t="shared" si="5"/>
-        <v>4.3956985532714032</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="6"/>
-        <v>30.95568988567743</v>
-      </c>
-      <c r="E30" s="3">
-        <f t="shared" si="7"/>
-        <v>496.52813650689097</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31">
-        <v>22</v>
-      </c>
-      <c r="B31" s="3">
-        <f t="shared" si="4"/>
-        <v>496.52813650689097</v>
-      </c>
-      <c r="C31" s="3">
-        <f t="shared" si="5"/>
-        <v>4.1377344708907584</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="6"/>
-        <v>31.213653968058072</v>
-      </c>
-      <c r="E31" s="3">
-        <f t="shared" si="7"/>
-        <v>465.31448253883292</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32">
-        <v>23</v>
-      </c>
-      <c r="B32" s="3">
-        <f t="shared" si="4"/>
-        <v>465.31448253883292</v>
-      </c>
-      <c r="C32" s="3">
-        <f t="shared" si="5"/>
-        <v>3.8776206878236077</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="6"/>
-        <v>31.473767751125223</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" si="7"/>
-        <v>433.84071478770773</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33">
-        <v>24</v>
-      </c>
-      <c r="B33" s="3">
-        <f t="shared" si="4"/>
-        <v>433.84071478770773</v>
-      </c>
-      <c r="C33" s="3">
-        <f t="shared" si="5"/>
-        <v>3.6153392898975643</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="6"/>
-        <v>31.736049149051269</v>
-      </c>
-      <c r="E33" s="8">
-        <f t="shared" si="7"/>
-        <v>402.10466563865646</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34">
-        <v>25</v>
-      </c>
-      <c r="B34" s="3">
-        <f t="shared" si="4"/>
-        <v>402.10466563865646</v>
-      </c>
-      <c r="C34" s="3">
-        <f t="shared" si="5"/>
-        <v>3.3508722136554705</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="6"/>
-        <v>32.00051622529336</v>
-      </c>
-      <c r="E34" s="3">
-        <f t="shared" si="7"/>
-        <v>370.10414941336307</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35">
-        <v>26</v>
-      </c>
-      <c r="B35" s="3">
-        <f t="shared" si="4"/>
-        <v>370.10414941336307</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" si="5"/>
-        <v>3.084201245111359</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="6"/>
-        <v>32.267187193837472</v>
-      </c>
-      <c r="E35" s="3">
-        <f t="shared" si="7"/>
-        <v>337.83696221952562</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36">
-        <v>27</v>
-      </c>
-      <c r="B36" s="3">
-        <f t="shared" si="4"/>
-        <v>337.83696221952562</v>
-      </c>
-      <c r="C36" s="3">
-        <f t="shared" si="5"/>
-        <v>2.8153080184960468</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="6"/>
-        <v>32.536080420452784</v>
-      </c>
-      <c r="E36" s="3">
-        <f t="shared" si="7"/>
-        <v>305.30088179907284</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37">
-        <v>28</v>
-      </c>
-      <c r="B37" s="3">
-        <f t="shared" si="4"/>
-        <v>305.30088179907284</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" si="5"/>
-        <v>2.5441740149922736</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="6"/>
-        <v>32.807214423956559</v>
-      </c>
-      <c r="E37" s="3">
-        <f t="shared" si="7"/>
-        <v>272.49366737511627</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38">
-        <v>29</v>
-      </c>
-      <c r="B38" s="3">
-        <f t="shared" si="4"/>
-        <v>272.49366737511627</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" si="5"/>
-        <v>2.2707805614593024</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="6"/>
-        <v>33.080607877489527</v>
-      </c>
-      <c r="E38" s="3">
-        <f t="shared" si="7"/>
-        <v>239.41305949762676</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39">
-        <v>30</v>
-      </c>
-      <c r="B39" s="3">
-        <f t="shared" si="4"/>
-        <v>239.41305949762676</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" si="5"/>
-        <v>1.9951088291468897</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="6"/>
-        <v>33.356279609801945</v>
-      </c>
-      <c r="E39" s="3">
-        <f t="shared" si="7"/>
-        <v>206.0567798878248</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40">
-        <v>31</v>
-      </c>
-      <c r="B40" s="3">
-        <f t="shared" si="4"/>
-        <v>206.0567798878248</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="5"/>
-        <v>1.7171398323985401</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="6"/>
-        <v>33.634248606550294</v>
-      </c>
-      <c r="E40" s="3">
-        <f t="shared" si="7"/>
-        <v>172.4225312812745</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41">
-        <v>32</v>
-      </c>
-      <c r="B41" s="3">
-        <f t="shared" ref="B41:B45" si="8">E40</f>
-        <v>172.4225312812745</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" ref="C41:C45" si="9">(B41*B$5)</f>
-        <v>1.4368544273439541</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" ref="D41:D45" si="10">MonthlyPayment-C41</f>
-        <v>33.914534011604879</v>
-      </c>
-      <c r="E41" s="3">
-        <f t="shared" ref="E41:E45" si="11">B41-D41</f>
-        <v>138.50799726966963</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42">
-        <v>33</v>
-      </c>
-      <c r="B42" s="3">
-        <f t="shared" si="8"/>
-        <v>138.50799726966963</v>
-      </c>
-      <c r="C42" s="3">
-        <f t="shared" si="9"/>
-        <v>1.1542333105805802</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="10"/>
-        <v>34.197155128368252</v>
-      </c>
-      <c r="E42" s="3">
-        <f t="shared" si="11"/>
-        <v>104.31084214130138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43">
-        <v>34</v>
-      </c>
-      <c r="B43" s="3">
-        <f t="shared" si="8"/>
-        <v>104.31084214130138</v>
-      </c>
-      <c r="C43" s="3">
-        <f t="shared" si="9"/>
-        <v>0.86925701784417819</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="10"/>
-        <v>34.482131421104654</v>
-      </c>
-      <c r="E43" s="3">
-        <f t="shared" si="11"/>
-        <v>69.828710720196725</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44">
-        <v>35</v>
-      </c>
-      <c r="B44" s="3">
-        <f t="shared" si="8"/>
-        <v>69.828710720196725</v>
-      </c>
-      <c r="C44" s="3">
-        <f t="shared" si="9"/>
-        <v>0.58190592266830599</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="10"/>
-        <v>34.769482516280526</v>
-      </c>
-      <c r="E44" s="3">
-        <f t="shared" si="11"/>
-        <v>35.059228203916199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45">
-        <v>36</v>
-      </c>
-      <c r="B45" s="3">
-        <f t="shared" si="8"/>
-        <v>35.059228203916199</v>
-      </c>
-      <c r="C45" s="3">
-        <f t="shared" si="9"/>
-        <v>0.292160235032635</v>
-      </c>
-      <c r="D45" s="3">
-        <f t="shared" si="10"/>
-        <v>35.059228203916199</v>
-      </c>
-      <c r="E45" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add loan amortizations to spreadsheet to cross-check results in the unit tests.
</commit_message>
<xml_diff>
--- a/Retirement SimulatorTests/MonthlyMortgageInterestCalculation.xlsx
+++ b/Retirement SimulatorTests/MonthlyMortgageInterestCalculation.xlsx
@@ -143,6 +143,64 @@
     <author>Steve Roehling</author>
   </authors>
   <commentList>
+    <comment ref="F22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Roehling:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Last payment before sim start, on 12/1/2011.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Roehling:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Starting balance set to 900.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Steve Roehling</author>
+  </authors>
+  <commentList>
     <comment ref="B5" authorId="0">
       <text>
         <r>
@@ -172,7 +230,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Steve Roehling</author>
@@ -230,7 +288,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Steve Roehling</author>
@@ -264,7 +322,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Steve Roehling</author>
@@ -981,10 +1039,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -1015,7 +1073,7 @@
       </c>
       <c r="B4" s="3">
         <f>F34</f>
-        <v>957.9389828676575</v>
+        <v>868.58607976761107</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1049,7 +1107,7 @@
       </c>
       <c r="B8" s="1">
         <f>-PMT(MonthlyInterestRate,NumPayments,LoanAmount,0,0)</f>
-        <v>30.909996480464986</v>
+        <v>28.026829629822963</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1328,7 +1386,7 @@
       <c r="E22" s="3">
         <v>10</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="8">
         <f t="shared" si="1"/>
         <v>980.88335852404032</v>
       </c>
@@ -1337,13 +1395,13 @@
       <c r="A23">
         <v>12</v>
       </c>
-      <c r="B23" s="1">
-        <f t="shared" si="0"/>
-        <v>980.88335852404032</v>
+      <c r="B23" s="16">
+        <f>B9</f>
+        <v>900</v>
       </c>
       <c r="C23" s="3">
         <f>(B23*B$6)</f>
-        <v>8.1740279877003363</v>
+        <v>7.5</v>
       </c>
       <c r="D23" s="3">
         <v>0</v>
@@ -1353,7 +1411,7 @@
       </c>
       <c r="F23" s="3">
         <f t="shared" si="1"/>
-        <v>979.05738651174067</v>
+        <v>897.5</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1362,11 +1420,11 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>979.05738651174067</v>
+        <v>897.5</v>
       </c>
       <c r="C24" s="3">
         <f>(B24*B$6)</f>
-        <v>8.1588115542645063</v>
+        <v>7.479166666666667</v>
       </c>
       <c r="D24" s="3">
         <v>0</v>
@@ -1376,7 +1434,7 @@
       </c>
       <c r="F24" s="3">
         <f t="shared" si="1"/>
-        <v>977.21619806600518</v>
+        <v>894.97916666666663</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1385,11 +1443,11 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>977.21619806600518</v>
+        <v>894.97916666666663</v>
       </c>
       <c r="C25" s="3">
         <f>(B25*B$6)</f>
-        <v>8.1434683172167102</v>
+        <v>7.4581597222222218</v>
       </c>
       <c r="D25" s="3">
         <v>0</v>
@@ -1399,7 +1457,7 @@
       </c>
       <c r="F25" s="3">
         <f t="shared" si="1"/>
-        <v>975.35966638322191</v>
+        <v>892.43732638888889</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1408,11 +1466,11 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>975.35966638322191</v>
+        <v>892.43732638888889</v>
       </c>
       <c r="C26" s="3">
         <f>(B26*B$6)</f>
-        <v>8.1279972198601822</v>
+        <v>7.4369777199074072</v>
       </c>
       <c r="D26" s="3">
         <v>0</v>
@@ -1422,7 +1480,7 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" si="1"/>
-        <v>973.48766360308207</v>
+        <v>889.87430410879631</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1431,11 +1489,11 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>973.48766360308207</v>
+        <v>889.87430410879631</v>
       </c>
       <c r="C27" s="3">
         <f>(B27*B$6)</f>
-        <v>8.1123971966923509</v>
+        <v>7.4156192009066357</v>
       </c>
       <c r="D27" s="3">
         <v>0</v>
@@ -1445,7 +1503,7 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" si="1"/>
-        <v>971.60006079977438</v>
+        <v>887.289923309703</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1454,11 +1512,11 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>971.60006079977438</v>
+        <v>887.289923309703</v>
       </c>
       <c r="C28" s="3">
         <f>(B28*B$6)</f>
-        <v>8.0966671733314524</v>
+        <v>7.3940826942475253</v>
       </c>
       <c r="D28" s="3">
         <v>0</v>
@@ -1468,7 +1526,7 @@
       </c>
       <c r="F28" s="3">
         <f t="shared" si="1"/>
-        <v>969.69672797310579</v>
+        <v>884.68400600395057</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1477,11 +1535,11 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>969.69672797310579</v>
+        <v>884.68400600395057</v>
       </c>
       <c r="C29" s="3">
         <f>(B29*B$6)</f>
-        <v>8.0808060664425483</v>
+        <v>7.3723667166995881</v>
       </c>
       <c r="D29" s="3">
         <v>0</v>
@@ -1491,7 +1549,7 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>967.7775340395483</v>
+        <v>882.05637272065019</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1500,11 +1558,11 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>967.7775340395483</v>
+        <v>882.05637272065019</v>
       </c>
       <c r="C30" s="3">
         <f>(B30*B$6)</f>
-        <v>8.0648127836629016</v>
+        <v>7.3504697726720849</v>
       </c>
       <c r="D30" s="3">
         <v>0</v>
@@ -1514,7 +1572,7 @@
       </c>
       <c r="F30" s="3">
         <f t="shared" si="1"/>
-        <v>965.84234682321119</v>
+        <v>879.4068424933223</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1523,11 +1581,11 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" si="0"/>
-        <v>965.84234682321119</v>
+        <v>879.4068424933223</v>
       </c>
       <c r="C31" s="3">
         <f>(B31*B$6)</f>
-        <v>8.0486862235267598</v>
+        <v>7.3283903541110194</v>
       </c>
       <c r="D31" s="3">
         <v>0</v>
@@ -1537,7 +1595,7 @@
       </c>
       <c r="F31" s="3">
         <f t="shared" si="1"/>
-        <v>963.8910330467379</v>
+        <v>876.73523284743328</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1546,11 +1604,11 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>963.8910330467379</v>
+        <v>876.73523284743328</v>
       </c>
       <c r="C32" s="3">
         <f>(B32*B$6)</f>
-        <v>8.0324252753894818</v>
+        <v>7.3061269403952771</v>
       </c>
       <c r="D32" s="3">
         <v>0</v>
@@ -1560,7 +1618,7 @@
       </c>
       <c r="F32" s="3">
         <f t="shared" si="1"/>
-        <v>961.92345832212743</v>
+        <v>874.04135978782858</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1569,11 +1627,11 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" si="0"/>
-        <v>961.92345832212743</v>
+        <v>874.04135978782858</v>
       </c>
       <c r="C33" s="3">
         <f>(B33*B$6)</f>
-        <v>8.016028819351062</v>
+        <v>7.2836779982319051</v>
       </c>
       <c r="D33" s="3">
         <v>0</v>
@@ -1583,7 +1641,7 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" si="1"/>
-        <v>959.93948714147848</v>
+        <v>871.32503778606053</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1592,11 +1650,11 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" si="0"/>
-        <v>959.93948714147848</v>
+        <v>871.32503778606053</v>
       </c>
       <c r="C34" s="3">
         <f>(B34*B$6)</f>
-        <v>7.9994957261789876</v>
+        <v>7.2610419815505045</v>
       </c>
       <c r="D34" s="3">
         <v>0</v>
@@ -1606,7 +1664,7 @@
       </c>
       <c r="F34" s="8">
         <f t="shared" si="1"/>
-        <v>957.9389828676575</v>
+        <v>868.58607976761107</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1633,24 +1691,24 @@
       <c r="A37" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="8">
         <f>F34</f>
-        <v>957.9389828676575</v>
+        <v>868.58607976761107</v>
       </c>
       <c r="C37" s="3">
         <f>(B37*B$6)</f>
-        <v>7.9828248572304794</v>
+        <v>7.2382173313967586</v>
       </c>
       <c r="D37" s="3">
         <f t="shared" ref="D37:D53" si="2">MonthlyPayment-C37</f>
-        <v>22.927171623234507</v>
+        <v>20.788612298426205</v>
       </c>
       <c r="E37" s="3">
         <v>10</v>
       </c>
       <c r="F37" s="3">
         <f>B37-SUM(D37:E37)</f>
-        <v>925.01181124442303</v>
+        <v>837.79746746918488</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1659,22 +1717,22 @@
       </c>
       <c r="B38" s="3">
         <f>F37</f>
-        <v>925.01181124442303</v>
+        <v>837.79746746918488</v>
       </c>
       <c r="C38" s="3">
         <f>(B38*B$6)</f>
-        <v>7.7084317603701917</v>
+        <v>6.981645562243207</v>
       </c>
       <c r="D38" s="3">
         <f t="shared" si="2"/>
-        <v>23.201564720094794</v>
+        <v>21.045184067579754</v>
       </c>
       <c r="E38" s="3">
         <v>10</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" ref="F38:F73" si="3">B38-SUM(D38:E38)</f>
-        <v>891.81024652432825</v>
+        <v>806.75228340160515</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1683,22 +1741,22 @@
       </c>
       <c r="B39" s="3">
         <f t="shared" ref="B39:B72" si="4">F38</f>
-        <v>891.81024652432825</v>
+        <v>806.75228340160515</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" ref="C39:C72" si="5">(B39*B$6)</f>
-        <v>7.4317520543694018</v>
+        <v>6.7229356950133763</v>
       </c>
       <c r="D39" s="3">
         <f t="shared" si="2"/>
-        <v>23.478244426095586</v>
+        <v>21.303893934809587</v>
       </c>
       <c r="E39" s="3">
         <v>10</v>
       </c>
       <c r="F39" s="3">
         <f t="shared" si="3"/>
-        <v>858.33200209823269</v>
+        <v>775.44838946679556</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1707,22 +1765,22 @@
       </c>
       <c r="B40" s="3">
         <f t="shared" si="4"/>
-        <v>858.33200209823269</v>
+        <v>775.44838946679556</v>
       </c>
       <c r="C40" s="3">
         <f t="shared" si="5"/>
-        <v>7.1527666841519393</v>
+        <v>6.4620699122232965</v>
       </c>
       <c r="D40" s="3">
         <f t="shared" si="2"/>
-        <v>23.757229796313048</v>
+        <v>21.564759717599667</v>
       </c>
       <c r="E40" s="3">
         <v>10</v>
       </c>
       <c r="F40" s="3">
         <f t="shared" si="3"/>
-        <v>824.57477230191967</v>
+        <v>743.88362974919585</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1731,22 +1789,22 @@
       </c>
       <c r="B41" s="3">
         <f t="shared" si="4"/>
-        <v>824.57477230191967</v>
+        <v>743.88362974919585</v>
       </c>
       <c r="C41" s="3">
         <f t="shared" si="5"/>
-        <v>6.8714564358493302</v>
+        <v>6.199030247909965</v>
       </c>
       <c r="D41" s="3">
         <f t="shared" si="2"/>
-        <v>24.038540044615658</v>
+        <v>21.827799381912996</v>
       </c>
       <c r="E41" s="3">
         <v>10</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="3"/>
-        <v>790.53623225730405</v>
+        <v>712.05583036728285</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1755,22 +1813,22 @@
       </c>
       <c r="B42" s="3">
         <f t="shared" si="4"/>
-        <v>790.53623225730405</v>
+        <v>712.05583036728285</v>
       </c>
       <c r="C42" s="3">
         <f t="shared" si="5"/>
-        <v>6.5878019354775335</v>
+        <v>5.9337985863940235</v>
       </c>
       <c r="D42" s="3">
         <f t="shared" si="2"/>
-        <v>24.322194544987454</v>
+        <v>22.09303104342894</v>
       </c>
       <c r="E42" s="3">
         <v>10</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="3"/>
-        <v>756.21403771231655</v>
+        <v>679.96279932385391</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1779,22 +1837,22 @@
       </c>
       <c r="B43" s="3">
         <f t="shared" si="4"/>
-        <v>756.21403771231655</v>
+        <v>679.96279932385391</v>
       </c>
       <c r="C43" s="3">
         <f t="shared" si="5"/>
-        <v>6.3017836476026377</v>
+        <v>5.6663566610321157</v>
       </c>
       <c r="D43" s="3">
         <f t="shared" si="2"/>
-        <v>24.60821283286235</v>
+        <v>22.360472968790848</v>
       </c>
       <c r="E43" s="3">
         <v>10</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" si="3"/>
-        <v>721.60582487945419</v>
+        <v>647.60232635506304</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1803,22 +1861,22 @@
       </c>
       <c r="B44" s="3">
         <f t="shared" si="4"/>
-        <v>721.60582487945419</v>
+        <v>647.60232635506304</v>
       </c>
       <c r="C44" s="3">
         <f t="shared" si="5"/>
-        <v>6.0133818739954519</v>
+        <v>5.3966860529588585</v>
       </c>
       <c r="D44" s="3">
         <f t="shared" si="2"/>
-        <v>24.896614606469534</v>
+        <v>22.630143576864103</v>
       </c>
       <c r="E44" s="3">
         <v>10</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" si="3"/>
-        <v>686.70921027298471</v>
+        <v>614.97218277819888</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1827,22 +1885,22 @@
       </c>
       <c r="B45" s="3">
         <f t="shared" si="4"/>
-        <v>686.70921027298471</v>
+        <v>614.97218277819888</v>
       </c>
       <c r="C45" s="3">
         <f t="shared" si="5"/>
-        <v>5.7225767522748727</v>
+        <v>5.1247681898183242</v>
       </c>
       <c r="D45" s="3">
         <f t="shared" si="2"/>
-        <v>25.187419728190115</v>
+        <v>22.902061440004637</v>
       </c>
       <c r="E45" s="3">
         <v>10</v>
       </c>
       <c r="F45" s="3">
         <f t="shared" si="3"/>
-        <v>651.52179054479461</v>
+        <v>582.07012133819421</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1851,22 +1909,22 @@
       </c>
       <c r="B46" s="3">
         <f t="shared" si="4"/>
-        <v>651.52179054479461</v>
+        <v>582.07012133819421</v>
       </c>
       <c r="C46" s="3">
         <f t="shared" si="5"/>
-        <v>5.4293482545399554</v>
+        <v>4.8505843444849521</v>
       </c>
       <c r="D46" s="3">
         <f t="shared" si="2"/>
-        <v>25.48064822592503</v>
+        <v>23.176245285338013</v>
       </c>
       <c r="E46" s="3">
         <v>10</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" si="3"/>
-        <v>616.04114231886956</v>
+        <v>548.89387605285617</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1875,22 +1933,22 @@
       </c>
       <c r="B47" s="3">
         <f t="shared" si="4"/>
-        <v>616.04114231886956</v>
+        <v>548.89387605285617</v>
       </c>
       <c r="C47" s="3">
         <f t="shared" si="5"/>
-        <v>5.1336761859905797</v>
+        <v>4.5741156337738014</v>
       </c>
       <c r="D47" s="3">
         <f t="shared" si="2"/>
-        <v>25.776320294474406</v>
+        <v>23.452713996049162</v>
       </c>
       <c r="E47" s="3">
         <v>10</v>
       </c>
       <c r="F47" s="3">
         <f t="shared" si="3"/>
-        <v>580.26482202439513</v>
+        <v>515.441162056807</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1899,22 +1957,22 @@
       </c>
       <c r="B48" s="3">
         <f t="shared" si="4"/>
-        <v>580.26482202439513</v>
+        <v>515.441162056807</v>
       </c>
       <c r="C48" s="3">
         <f t="shared" si="5"/>
-        <v>4.8355401835366258</v>
+        <v>4.2953430171400582</v>
       </c>
       <c r="D48" s="3">
         <f t="shared" si="2"/>
-        <v>26.074456296928361</v>
+        <v>23.731486612682904</v>
       </c>
       <c r="E48" s="3">
         <v>10</v>
       </c>
       <c r="F48" s="8">
         <f t="shared" si="3"/>
-        <v>544.19036572746677</v>
+        <v>481.70967544412412</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>33</v>
@@ -1926,22 +1984,22 @@
       </c>
       <c r="B49" s="3">
         <f t="shared" si="4"/>
-        <v>544.19036572746677</v>
+        <v>481.70967544412412</v>
       </c>
       <c r="C49" s="3">
         <f t="shared" si="5"/>
-        <v>4.5349197143955564</v>
+        <v>4.0142472953677011</v>
       </c>
       <c r="D49" s="3">
         <f t="shared" si="2"/>
-        <v>26.37507676606943</v>
+        <v>24.01258233445526</v>
       </c>
       <c r="E49" s="3">
         <v>10</v>
       </c>
       <c r="F49" s="3">
         <f t="shared" si="3"/>
-        <v>507.81528896139736</v>
+        <v>447.69709310966886</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1950,22 +2008,22 @@
       </c>
       <c r="B50" s="3">
         <f t="shared" si="4"/>
-        <v>507.81528896139736</v>
+        <v>447.69709310966886</v>
       </c>
       <c r="C50" s="3">
         <f t="shared" si="5"/>
-        <v>4.2317940746783114</v>
+        <v>3.7308091092472404</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" si="2"/>
-        <v>26.678202405786674</v>
+        <v>24.296020520575723</v>
       </c>
       <c r="E50" s="3">
         <v>10</v>
       </c>
       <c r="F50" s="3">
         <f t="shared" si="3"/>
-        <v>471.13708655561067</v>
+        <v>413.40107258909313</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1974,22 +2032,22 @@
       </c>
       <c r="B51" s="3">
         <f t="shared" si="4"/>
-        <v>471.13708655561067</v>
+        <v>413.40107258909313</v>
       </c>
       <c r="C51" s="3">
         <f t="shared" si="5"/>
-        <v>3.9261423879634223</v>
+        <v>3.4450089382424429</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" si="2"/>
-        <v>26.983854092501563</v>
+        <v>24.581820691580521</v>
       </c>
       <c r="E51" s="3">
         <v>10</v>
       </c>
       <c r="F51" s="3">
         <f t="shared" si="3"/>
-        <v>434.15323246310913</v>
+        <v>378.81925189751263</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1998,22 +2056,22 @@
       </c>
       <c r="B52" s="3">
         <f t="shared" si="4"/>
-        <v>434.15323246310913</v>
+        <v>378.81925189751263</v>
       </c>
       <c r="C52" s="3">
         <f t="shared" si="5"/>
-        <v>3.6179436038592425</v>
+        <v>3.1568270991459384</v>
       </c>
       <c r="D52" s="3">
         <f t="shared" si="2"/>
-        <v>27.292052876605744</v>
+        <v>24.870002530677024</v>
       </c>
       <c r="E52" s="3">
         <v>10</v>
       </c>
       <c r="F52" s="3">
         <f t="shared" si="3"/>
-        <v>396.8611795865034</v>
+        <v>343.9492493668356</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2022,22 +2080,22 @@
       </c>
       <c r="B53" s="3">
         <f t="shared" si="4"/>
-        <v>396.8611795865034</v>
+        <v>343.9492493668356</v>
       </c>
       <c r="C53" s="3">
         <f t="shared" si="5"/>
-        <v>3.3071764965541948</v>
+        <v>2.8662437447236302</v>
       </c>
       <c r="D53" s="3">
         <f t="shared" si="2"/>
-        <v>27.602819983910791</v>
+        <v>25.160585885099334</v>
       </c>
       <c r="E53" s="3">
         <v>10</v>
       </c>
       <c r="F53" s="3">
         <f t="shared" si="3"/>
-        <v>359.25835960259258</v>
+        <v>308.78866348173625</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2046,22 +2104,22 @@
       </c>
       <c r="B54" s="3">
         <f t="shared" si="4"/>
-        <v>359.25835960259258</v>
+        <v>308.78866348173625</v>
       </c>
       <c r="C54" s="3">
         <f t="shared" si="5"/>
-        <v>2.9938196633549383</v>
+        <v>2.573238862347802</v>
       </c>
       <c r="D54" s="3">
         <f t="shared" ref="D54:D67" si="6">MonthlyPayment-C54</f>
-        <v>27.916176817110049</v>
+        <v>25.453590767475163</v>
       </c>
       <c r="E54" s="3">
         <v>10</v>
       </c>
       <c r="F54" s="3">
         <f t="shared" si="3"/>
-        <v>321.34218278548252</v>
+        <v>273.33507271426106</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2070,22 +2128,22 @@
       </c>
       <c r="B55" s="3">
         <f t="shared" si="4"/>
-        <v>321.34218278548252</v>
+        <v>273.33507271426106</v>
       </c>
       <c r="C55" s="3">
         <f t="shared" si="5"/>
-        <v>2.6778515232123543</v>
+        <v>2.277792272618842</v>
       </c>
       <c r="D55" s="3">
         <f t="shared" si="6"/>
-        <v>28.232144957252633</v>
+        <v>25.74903735720412</v>
       </c>
       <c r="E55" s="3">
         <v>10</v>
       </c>
       <c r="F55" s="3">
         <f t="shared" si="3"/>
-        <v>283.11003782822991</v>
+        <v>237.58603535705694</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2094,22 +2152,22 @@
       </c>
       <c r="B56" s="3">
         <f t="shared" si="4"/>
-        <v>283.11003782822991</v>
+        <v>237.58603535705694</v>
       </c>
       <c r="C56" s="3">
         <f t="shared" si="5"/>
-        <v>2.3592503152352493</v>
+        <v>1.9798836279754746</v>
       </c>
       <c r="D56" s="3">
         <f t="shared" si="6"/>
-        <v>28.550746165229736</v>
+        <v>26.046946001847488</v>
       </c>
       <c r="E56" s="3">
         <v>10</v>
       </c>
       <c r="F56" s="3">
         <f t="shared" si="3"/>
-        <v>244.55929166300018</v>
+        <v>201.53908935520946</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2118,22 +2176,22 @@
       </c>
       <c r="B57" s="3">
         <f t="shared" si="4"/>
-        <v>244.55929166300018</v>
+        <v>201.53908935520946</v>
       </c>
       <c r="C57" s="3">
         <f t="shared" si="5"/>
-        <v>2.0379940971916684</v>
+        <v>1.6794924112934122</v>
       </c>
       <c r="D57" s="3">
         <f t="shared" si="6"/>
-        <v>28.872002383273319</v>
+        <v>26.34733721852955</v>
       </c>
       <c r="E57" s="3">
         <v>10</v>
       </c>
       <c r="F57" s="3">
         <f t="shared" si="3"/>
-        <v>205.68728927972685</v>
+        <v>165.1917521366799</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2142,22 +2200,22 @@
       </c>
       <c r="B58" s="3">
         <f t="shared" si="4"/>
-        <v>205.68728927972685</v>
+        <v>165.1917521366799</v>
       </c>
       <c r="C58" s="3">
         <f t="shared" si="5"/>
-        <v>1.7140607439977238</v>
+        <v>1.3765979344723325</v>
       </c>
       <c r="D58" s="3">
         <f t="shared" si="6"/>
-        <v>29.195935736467263</v>
+        <v>26.65023169535063</v>
       </c>
       <c r="E58" s="3">
         <v>10</v>
       </c>
       <c r="F58" s="3">
         <f t="shared" si="3"/>
-        <v>166.49135354325961</v>
+        <v>128.54152044132928</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2166,22 +2224,22 @@
       </c>
       <c r="B59" s="3">
         <f t="shared" si="4"/>
-        <v>166.49135354325961</v>
+        <v>128.54152044132928</v>
       </c>
       <c r="C59" s="3">
         <f t="shared" si="5"/>
-        <v>1.3874279461938301</v>
+        <v>1.0711793370110774</v>
       </c>
       <c r="D59" s="3">
         <f t="shared" si="6"/>
-        <v>29.522568534271155</v>
+        <v>26.955650292811885</v>
       </c>
       <c r="E59" s="3">
         <v>10</v>
       </c>
       <c r="F59" s="3">
         <f t="shared" si="3"/>
-        <v>126.96878500898845</v>
+        <v>91.585870148517401</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2190,22 +2248,22 @@
       </c>
       <c r="B60" s="3">
         <f t="shared" si="4"/>
-        <v>126.96878500898845</v>
+        <v>91.585870148517401</v>
       </c>
       <c r="C60" s="3">
         <f t="shared" si="5"/>
-        <v>1.0580732084082372</v>
+        <v>0.76321558457097838</v>
       </c>
       <c r="D60" s="3">
         <f t="shared" si="6"/>
-        <v>29.851923272056748</v>
+        <v>27.263614045251984</v>
       </c>
       <c r="E60" s="3">
         <v>10</v>
       </c>
       <c r="F60" s="8">
         <f t="shared" si="3"/>
-        <v>87.116861736931696</v>
+        <v>54.322256103265417</v>
       </c>
       <c r="G60" s="9" t="s">
         <v>20</v>
@@ -2217,22 +2275,22 @@
       </c>
       <c r="B61" s="3">
         <f t="shared" si="4"/>
-        <v>87.116861736931696</v>
+        <v>54.322256103265417</v>
       </c>
       <c r="C61" s="3">
         <f t="shared" si="5"/>
-        <v>0.72597384780776408</v>
+        <v>0.45268546752721178</v>
       </c>
       <c r="D61" s="3">
         <f t="shared" si="6"/>
-        <v>30.184022632657221</v>
+        <v>27.574144162295752</v>
       </c>
       <c r="E61" s="3">
         <v>10</v>
       </c>
       <c r="F61" s="3">
         <f t="shared" si="3"/>
-        <v>46.932839104274478</v>
+        <v>16.748111940969665</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2241,22 +2299,22 @@
       </c>
       <c r="B62" s="3">
         <f t="shared" si="4"/>
-        <v>46.932839104274478</v>
+        <v>16.748111940969665</v>
       </c>
       <c r="C62" s="3">
         <f t="shared" si="5"/>
-        <v>0.39110699253562065</v>
+        <v>0.13956759950808054</v>
       </c>
       <c r="D62" s="3">
         <f t="shared" si="6"/>
-        <v>30.518889487929364</v>
+        <v>27.887262030314883</v>
       </c>
       <c r="E62" s="3">
         <v>10</v>
       </c>
       <c r="F62" s="3">
         <f t="shared" si="3"/>
-        <v>6.4139496163451142</v>
+        <v>-21.139150089345222</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2265,22 +2323,22 @@
       </c>
       <c r="B63" s="3">
         <f t="shared" si="4"/>
-        <v>6.4139496163451142</v>
+        <v>-21.139150089345222</v>
       </c>
       <c r="C63" s="3">
         <f t="shared" si="5"/>
-        <v>5.3449580136209283E-2</v>
+        <v>-0.17615958407787685</v>
       </c>
       <c r="D63" s="3">
         <f t="shared" si="6"/>
-        <v>30.856546900328777</v>
+        <v>28.202989213900839</v>
       </c>
       <c r="E63" s="3">
         <v>10</v>
       </c>
       <c r="F63" s="3">
         <f t="shared" si="3"/>
-        <v>-34.442597283983666</v>
+        <v>-59.342139303246057</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2289,22 +2347,22 @@
       </c>
       <c r="B64" s="3">
         <f t="shared" si="4"/>
-        <v>-34.442597283983666</v>
+        <v>-59.342139303246057</v>
       </c>
       <c r="C64" s="3">
         <f t="shared" si="5"/>
-        <v>-0.28702164403319719</v>
+        <v>-0.49451782752705048</v>
       </c>
       <c r="D64" s="3">
         <f t="shared" si="6"/>
-        <v>31.197018124498182</v>
+        <v>28.521347457350014</v>
       </c>
       <c r="E64" s="3">
         <v>10</v>
       </c>
       <c r="F64" s="3">
         <f t="shared" si="3"/>
-        <v>-75.639615408481859</v>
+        <v>-97.863486760596075</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2313,22 +2371,22 @@
       </c>
       <c r="B65" s="3">
         <f t="shared" si="4"/>
-        <v>-75.639615408481859</v>
+        <v>-97.863486760596075</v>
       </c>
       <c r="C65" s="3">
         <f t="shared" si="5"/>
-        <v>-0.63033012840401548</v>
+        <v>-0.81552905633830064</v>
       </c>
       <c r="D65" s="3">
         <f t="shared" si="6"/>
-        <v>31.540326608869002</v>
+        <v>28.842358686161262</v>
       </c>
       <c r="E65" s="3">
         <v>10</v>
       </c>
       <c r="F65" s="3">
         <f t="shared" si="3"/>
-        <v>-117.17994201735087</v>
+        <v>-136.70584544675734</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2337,22 +2395,22 @@
       </c>
       <c r="B66" s="3">
         <f t="shared" si="4"/>
-        <v>-117.17994201735087</v>
+        <v>-136.70584544675734</v>
       </c>
       <c r="C66" s="3">
         <f t="shared" si="5"/>
-        <v>-0.97649951681125724</v>
+        <v>-1.1392153787229777</v>
       </c>
       <c r="D66" s="3">
         <f t="shared" si="6"/>
-        <v>31.886495997276242</v>
+        <v>29.16604500854594</v>
       </c>
       <c r="E66" s="3">
         <v>10</v>
       </c>
       <c r="F66" s="3">
         <f t="shared" si="3"/>
-        <v>-159.06643801462712</v>
+        <v>-175.87189045530329</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2361,22 +2419,22 @@
       </c>
       <c r="B67" s="3">
         <f t="shared" si="4"/>
-        <v>-159.06643801462712</v>
+        <v>-175.87189045530329</v>
       </c>
       <c r="C67" s="3">
         <f t="shared" si="5"/>
-        <v>-1.3255536501218927</v>
+        <v>-1.4655990871275273</v>
       </c>
       <c r="D67" s="3">
         <f t="shared" si="6"/>
-        <v>32.23555013058688</v>
+        <v>29.492428716950489</v>
       </c>
       <c r="E67" s="3">
         <v>10</v>
       </c>
       <c r="F67" s="3">
         <f t="shared" si="3"/>
-        <v>-201.30198814521401</v>
+        <v>-215.36431917225377</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2385,22 +2443,22 @@
       </c>
       <c r="B68" s="3">
         <f t="shared" si="4"/>
-        <v>-201.30198814521401</v>
+        <v>-215.36431917225377</v>
       </c>
       <c r="C68" s="3">
         <f t="shared" si="5"/>
-        <v>-1.6775165678767834</v>
+        <v>-1.7947026597687814</v>
       </c>
       <c r="D68" s="3">
         <f t="shared" ref="D68:D72" si="7">MonthlyPayment-C68</f>
-        <v>32.587513048341769</v>
+        <v>29.821532289591744</v>
       </c>
       <c r="E68" s="3">
         <v>10</v>
       </c>
       <c r="F68" s="3">
         <f t="shared" si="3"/>
-        <v>-243.88950119355579</v>
+        <v>-255.18585146184552</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2409,22 +2467,22 @@
       </c>
       <c r="B69" s="3">
         <f t="shared" si="4"/>
-        <v>-243.88950119355579</v>
+        <v>-255.18585146184552</v>
       </c>
       <c r="C69" s="3">
         <f t="shared" si="5"/>
-        <v>-2.0324125099462984</v>
+        <v>-2.126548762182046</v>
       </c>
       <c r="D69" s="3">
         <f t="shared" si="7"/>
-        <v>32.942408990411288</v>
+        <v>30.15337839200501</v>
       </c>
       <c r="E69" s="3">
         <v>10</v>
       </c>
       <c r="F69" s="3">
         <f t="shared" si="3"/>
-        <v>-286.83191018396707</v>
+        <v>-295.3392298538505</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2433,22 +2491,22 @@
       </c>
       <c r="B70" s="3">
         <f t="shared" si="4"/>
-        <v>-286.83191018396707</v>
+        <v>-295.3392298538505</v>
       </c>
       <c r="C70" s="3">
         <f t="shared" si="5"/>
-        <v>-2.3902659181997254</v>
+        <v>-2.4611602487820874</v>
       </c>
       <c r="D70" s="3">
         <f t="shared" si="7"/>
-        <v>33.300262398664714</v>
+        <v>30.487989878605049</v>
       </c>
       <c r="E70" s="3">
         <v>10</v>
       </c>
       <c r="F70" s="3">
         <f t="shared" si="3"/>
-        <v>-330.13217258263177</v>
+        <v>-335.82721973245555</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2457,22 +2515,22 @@
       </c>
       <c r="B71" s="3">
         <f t="shared" si="4"/>
-        <v>-330.13217258263177</v>
+        <v>-335.82721973245555</v>
       </c>
       <c r="C71" s="3">
         <f t="shared" si="5"/>
-        <v>-2.7511014381885981</v>
+        <v>-2.7985601644371294</v>
       </c>
       <c r="D71" s="3">
         <f t="shared" si="7"/>
-        <v>33.661097918653581</v>
+        <v>30.825389794260094</v>
       </c>
       <c r="E71" s="3">
         <v>10</v>
       </c>
       <c r="F71" s="3">
         <f t="shared" si="3"/>
-        <v>-373.79327050128535</v>
+        <v>-376.65260952671565</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2481,22 +2539,22 @@
       </c>
       <c r="B72" s="3">
         <f t="shared" si="4"/>
-        <v>-373.79327050128535</v>
+        <v>-376.65260952671565</v>
       </c>
       <c r="C72" s="3">
         <f t="shared" si="5"/>
-        <v>-3.1149439208440444</v>
+        <v>-3.1387717460559639</v>
       </c>
       <c r="D72" s="3">
         <f t="shared" si="7"/>
-        <v>34.024940401309031</v>
+        <v>31.165601375878929</v>
       </c>
       <c r="E72" s="3">
         <v>10</v>
       </c>
       <c r="F72" s="3">
         <f t="shared" si="3"/>
-        <v>-417.81821090259439</v>
+        <v>-417.81821090259456</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2508,6 +2566,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add unit tests for variable loan interest rates (ARMs)
The tests were of the PeriodInterestBearingWorkingBalance class, which is leveraged for loan interest and payment calculations. This testing uncovered a defect in this class, which has been fixed and tested with these changes.
</commit_message>
<xml_diff>
--- a/Retirement SimulatorTests/MonthlyMortgageInterestCalculation.xlsx
+++ b/Retirement SimulatorTests/MonthlyMortgageInterestCalculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22040" yWindow="1760" windowWidth="28720" windowHeight="17100" tabRatio="823" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="6180" yWindow="1180" windowWidth="20100" windowHeight="18480" tabRatio="823" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Deferred Future Loan UT (8)" sheetId="15" r:id="rId1"/>
@@ -21,13 +21,17 @@
     <sheet name="testFutureLoan02 unit test" sheetId="2" r:id="rId12"/>
     <sheet name="Deferred Future Loan UT (2)" sheetId="5" r:id="rId13"/>
     <sheet name="Deferred Future Loan UT" sheetId="4" r:id="rId14"/>
-    <sheet name="ARM" sheetId="13" r:id="rId15"/>
+    <sheet name="ARM Scratch" sheetId="13" r:id="rId15"/>
+    <sheet name="ARM UT 1" sheetId="16" r:id="rId16"/>
+    <sheet name="ARM UT 2" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="AdjustedAnnualRate">'Early Payoff'!$B$8</definedName>
     <definedName name="AjustedAnnualRate">'Early Payoff'!$B$8</definedName>
     <definedName name="DailyRate">'Early Payoff'!$B$9</definedName>
-    <definedName name="DeferMonths" localSheetId="14">ARM!$G$5</definedName>
+    <definedName name="DeferMonths" localSheetId="14">'ARM Scratch'!$G$5</definedName>
+    <definedName name="DeferMonths" localSheetId="15">'ARM UT 1'!$G$5</definedName>
+    <definedName name="DeferMonths" localSheetId="16">'ARM UT 2'!$G$5</definedName>
     <definedName name="DeferMonths" localSheetId="12">'Deferred Future Loan UT (2)'!$F$5</definedName>
     <definedName name="DeferMonths" localSheetId="8">'Deferred Future Loan UT (3)'!$F$5</definedName>
     <definedName name="DeferMonths" localSheetId="7">'Deferred Future Loan UT (4)'!$F$5</definedName>
@@ -36,7 +40,9 @@
     <definedName name="DeferMonths" localSheetId="0">'Deferred Future Loan UT (8)'!$G$6</definedName>
     <definedName name="DeferMonths" localSheetId="1">'Past Loan Extra Pmt Init Bal'!$G$6</definedName>
     <definedName name="DeferMonths">'Deferred Future Loan UT'!$F$5</definedName>
-    <definedName name="InterestRate" localSheetId="14">ARM!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="14">'ARM Scratch'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="15">'ARM UT 1'!$B$4</definedName>
+    <definedName name="InterestRate" localSheetId="16">'ARM UT 2'!$B$4</definedName>
     <definedName name="InterestRate" localSheetId="4">'Deferred Extra Pmt'!$B$6</definedName>
     <definedName name="InterestRate" localSheetId="13">'Deferred Future Loan UT'!$B$4</definedName>
     <definedName name="InterestRate" localSheetId="12">'Deferred Future Loan UT (2)'!$B$4</definedName>
@@ -51,8 +57,12 @@
     <definedName name="InterestRate" localSheetId="11">'testFutureLoan02 unit test'!$B$2</definedName>
     <definedName name="InterestRate" localSheetId="10">'testSimpleLoan unit test'!$B$2</definedName>
     <definedName name="InterestRate">'Scratchpad for Testing'!$B$2</definedName>
-    <definedName name="InterestRateAfterRateAdjust">ARM!$C$5</definedName>
-    <definedName name="Loan_Amount" localSheetId="14">ARM!$A$3</definedName>
+    <definedName name="InterestRateAfterRateAdjust" localSheetId="15">'ARM UT 1'!$C$5</definedName>
+    <definedName name="InterestRateAfterRateAdjust" localSheetId="16">'ARM UT 2'!$D$5</definedName>
+    <definedName name="InterestRateAfterRateAdjust">'ARM Scratch'!$C$5</definedName>
+    <definedName name="Loan_Amount" localSheetId="14">'ARM Scratch'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="15">'ARM UT 1'!$A$3</definedName>
+    <definedName name="Loan_Amount" localSheetId="16">'ARM UT 2'!$A$3</definedName>
     <definedName name="Loan_Amount" localSheetId="4">'Deferred Extra Pmt'!$A$5</definedName>
     <definedName name="Loan_Amount" localSheetId="13">'Deferred Future Loan UT'!$A$3</definedName>
     <definedName name="Loan_Amount" localSheetId="12">'Deferred Future Loan UT (2)'!$A$3</definedName>
@@ -67,7 +77,9 @@
     <definedName name="Loan_Amount" localSheetId="11">'testFutureLoan02 unit test'!$A$1</definedName>
     <definedName name="Loan_Amount" localSheetId="10">'testSimpleLoan unit test'!$A$1</definedName>
     <definedName name="Loan_Amount">'Scratchpad for Testing'!$A$1</definedName>
-    <definedName name="LoanAmount" localSheetId="14">ARM!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="14">'ARM Scratch'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="15">'ARM UT 1'!$B$3</definedName>
+    <definedName name="LoanAmount" localSheetId="16">'ARM UT 2'!$B$3</definedName>
     <definedName name="LoanAmount" localSheetId="4">'Deferred Extra Pmt'!$B$5</definedName>
     <definedName name="LoanAmount" localSheetId="13">'Deferred Future Loan UT'!$B$3</definedName>
     <definedName name="LoanAmount" localSheetId="12">'Deferred Future Loan UT (2)'!$B$3</definedName>
@@ -82,7 +94,9 @@
     <definedName name="LoanAmount" localSheetId="11">'testFutureLoan02 unit test'!$B$1</definedName>
     <definedName name="LoanAmount" localSheetId="10">'testSimpleLoan unit test'!$B$1</definedName>
     <definedName name="LoanAmount">'Scratchpad for Testing'!$B$1</definedName>
-    <definedName name="MonthlyInterestRate" localSheetId="14">ARM!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="14">'ARM Scratch'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="15">'ARM UT 1'!$B$5</definedName>
+    <definedName name="MonthlyInterestRate" localSheetId="16">'ARM UT 2'!$B$5</definedName>
     <definedName name="MonthlyInterestRate" localSheetId="4">'Deferred Extra Pmt'!$B$7</definedName>
     <definedName name="MonthlyInterestRate" localSheetId="13">'Deferred Future Loan UT'!$B$5</definedName>
     <definedName name="MonthlyInterestRate" localSheetId="12">'Deferred Future Loan UT (2)'!$B$5</definedName>
@@ -97,7 +111,9 @@
     <definedName name="MonthlyInterestRate" localSheetId="11">'testFutureLoan02 unit test'!$B$3</definedName>
     <definedName name="MonthlyInterestRate" localSheetId="10">'testSimpleLoan unit test'!$B$3</definedName>
     <definedName name="MonthlyInterestRate">'Scratchpad for Testing'!$B$3</definedName>
-    <definedName name="MonthlyMultiplier" localSheetId="14">ARM!$G$3</definedName>
+    <definedName name="MonthlyMultiplier" localSheetId="14">'ARM Scratch'!$G$3</definedName>
+    <definedName name="MonthlyMultiplier" localSheetId="15">'ARM UT 1'!$G$3</definedName>
+    <definedName name="MonthlyMultiplier" localSheetId="16">'ARM UT 2'!$G$3</definedName>
     <definedName name="MonthlyMultiplier" localSheetId="12">'Deferred Future Loan UT (2)'!$F$3</definedName>
     <definedName name="MonthlyMultiplier" localSheetId="8">'Deferred Future Loan UT (3)'!$F$3</definedName>
     <definedName name="MonthlyMultiplier" localSheetId="7">'Deferred Future Loan UT (4)'!$F$3</definedName>
@@ -106,7 +122,9 @@
     <definedName name="MonthlyMultiplier" localSheetId="0">'Deferred Future Loan UT (8)'!$G$4</definedName>
     <definedName name="MonthlyMultiplier" localSheetId="1">'Past Loan Extra Pmt Init Bal'!$G$4</definedName>
     <definedName name="MonthlyMultiplier">'Deferred Future Loan UT'!$F$3</definedName>
-    <definedName name="MonthlyPayment" localSheetId="14">ARM!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="14">'ARM Scratch'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="15">'ARM UT 1'!$B$7</definedName>
+    <definedName name="MonthlyPayment" localSheetId="16">'ARM UT 2'!$B$7</definedName>
     <definedName name="MonthlyPayment" localSheetId="4">'Deferred Extra Pmt'!$B$9</definedName>
     <definedName name="MonthlyPayment" localSheetId="13">'Deferred Future Loan UT'!$B$7</definedName>
     <definedName name="MonthlyPayment" localSheetId="12">'Deferred Future Loan UT (2)'!$B$7</definedName>
@@ -121,8 +139,12 @@
     <definedName name="MonthlyPayment" localSheetId="11">'testFutureLoan02 unit test'!$B$5</definedName>
     <definedName name="MonthlyPayment" localSheetId="10">'testSimpleLoan unit test'!$B$5</definedName>
     <definedName name="MonthlyPayment">'Scratchpad for Testing'!$B$5</definedName>
-    <definedName name="MonthlyPaymentAfterRateAdjust">ARM!$C$7</definedName>
-    <definedName name="NumPayments" localSheetId="14">ARM!$B$6</definedName>
+    <definedName name="MonthlyPaymentAfterRateAdjust" localSheetId="15">'ARM UT 1'!$C$7</definedName>
+    <definedName name="MonthlyPaymentAfterRateAdjust" localSheetId="16">'ARM UT 2'!$D$7</definedName>
+    <definedName name="MonthlyPaymentAfterRateAdjust">'ARM Scratch'!$C$7</definedName>
+    <definedName name="NumPayments" localSheetId="14">'ARM Scratch'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="15">'ARM UT 1'!$B$6</definedName>
+    <definedName name="NumPayments" localSheetId="16">'ARM UT 2'!$B$6</definedName>
     <definedName name="NumPayments" localSheetId="4">'Deferred Extra Pmt'!$B$8</definedName>
     <definedName name="NumPayments" localSheetId="13">'Deferred Future Loan UT'!$B$6</definedName>
     <definedName name="NumPayments" localSheetId="12">'Deferred Future Loan UT (2)'!$B$6</definedName>
@@ -139,7 +161,7 @@
     <definedName name="NumPayments">'Scratchpad for Testing'!$B$4</definedName>
     <definedName name="ProratedDays">'Early Payoff'!$B$11</definedName>
   </definedNames>
-  <calcPr calcId="140000" calcCompleted="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -426,7 +448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="77">
   <si>
     <t>Interest Rate</t>
   </si>
@@ -646,6 +668,18 @@
   <si>
     <t>Adjusted at Month 37</t>
   </si>
+  <si>
+    <t>Adjusted at Month 11</t>
+  </si>
+  <si>
+    <t>testPeriodicInterestBearingBal (WorkingBalanceTest.m)</t>
+  </si>
+  <si>
+    <t>After Deferment</t>
+  </si>
+  <si>
+    <t>testPeriodicInterestBearingBal,testPeriodicInterestBearingBalWithInterestOnlyPayment (WorkingBalanceTest.m)</t>
+  </si>
 </sst>
 </file>
 
@@ -732,7 +766,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -759,6 +793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6844,8 +6879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6881,10 +6916,10 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="26">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="26">
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
@@ -7011,15 +7046,15 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" ref="B13:B70" si="3">F12</f>
+        <f t="shared" ref="B13:B47" si="3">F12</f>
         <v>149753.37528429631</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" ref="C13:C70" si="4">(B13*B$5)</f>
+        <f t="shared" ref="C13:C46" si="4">(B13*B$5)</f>
         <v>873.56135582506192</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ref="D13:D70" si="5">MonthlyPayment-C13</f>
+        <f t="shared" ref="D13:D46" si="5">MonthlyPayment-C13</f>
         <v>124.39238694371295</v>
       </c>
       <c r="E13" s="3">
@@ -7027,7 +7062,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" ref="F13:F70" si="6">B13-SUM(D13:E13)</f>
+        <f t="shared" ref="F13:F47" si="6">B13-SUM(D13:E13)</f>
         <v>149628.9828973526</v>
       </c>
     </row>
@@ -7865,11 +7900,11 @@
         <v>145090.44466853084</v>
       </c>
       <c r="C47" s="7">
-        <f>(B47*InterestRateAfterRateAdjust)</f>
+        <f t="shared" ref="C47:C70" si="7">(B47*InterestRateAfterRateAdjust)</f>
         <v>876.58810320570717</v>
       </c>
       <c r="D47" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C47</f>
+        <f t="shared" ref="D47:D70" si="8">MonthlyPaymentAfterRateAdjust-C47</f>
         <v>145.13009860879254</v>
       </c>
       <c r="E47" s="7">
@@ -7886,23 +7921,23 @@
         <v>38</v>
       </c>
       <c r="B48" s="7">
-        <f t="shared" ref="B48:B70" si="7">F47</f>
+        <f t="shared" ref="B48:B70" si="9">F47</f>
         <v>144945.31456992205</v>
       </c>
       <c r="C48" s="7">
-        <f>(B48*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>875.71127552661233</v>
       </c>
       <c r="D48" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C48</f>
+        <f t="shared" si="8"/>
         <v>146.00692628788738</v>
       </c>
       <c r="E48" s="7">
-        <f t="shared" ref="E48:E70" si="8">C$8</f>
+        <f t="shared" ref="E48:E70" si="10">C$8</f>
         <v>0</v>
       </c>
       <c r="F48" s="7">
-        <f t="shared" ref="F48:F70" si="9">B48-SUM(D48:E48)</f>
+        <f t="shared" ref="F48:F70" si="11">B48-SUM(D48:E48)</f>
         <v>144799.30764363415</v>
       </c>
     </row>
@@ -7911,23 +7946,23 @@
         <v>39</v>
       </c>
       <c r="B49" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>144799.30764363415</v>
       </c>
       <c r="C49" s="7">
-        <f>(B49*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>874.82915034695634</v>
       </c>
       <c r="D49" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C49</f>
+        <f t="shared" si="8"/>
         <v>146.88905146754337</v>
       </c>
       <c r="E49" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F49" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>144652.41859216662</v>
       </c>
     </row>
@@ -7936,23 +7971,23 @@
         <v>40</v>
       </c>
       <c r="B50" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>144652.41859216662</v>
       </c>
       <c r="C50" s="7">
-        <f>(B50*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>873.94169566100663</v>
       </c>
       <c r="D50" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C50</f>
+        <f t="shared" si="8"/>
         <v>147.77650615349307</v>
       </c>
       <c r="E50" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F50" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>144504.64208601313</v>
       </c>
     </row>
@@ -7961,23 +7996,23 @@
         <v>41</v>
       </c>
       <c r="B51" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>144504.64208601313</v>
       </c>
       <c r="C51" s="7">
-        <f>(B51*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>873.04887926966262</v>
       </c>
       <c r="D51" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C51</f>
+        <f t="shared" si="8"/>
         <v>148.66932254483709</v>
       </c>
       <c r="E51" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F51" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>144355.97276346831</v>
       </c>
     </row>
@@ -7986,23 +8021,23 @@
         <v>42</v>
       </c>
       <c r="B52" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>144355.97276346831</v>
       </c>
       <c r="C52" s="7">
-        <f>(B52*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>872.15066877928768</v>
       </c>
       <c r="D52" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C52</f>
+        <f t="shared" si="8"/>
         <v>149.56753303521202</v>
       </c>
       <c r="E52" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F52" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>144206.4052304331</v>
       </c>
     </row>
@@ -8011,23 +8046,23 @@
         <v>43</v>
       </c>
       <c r="B53" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>144206.4052304331</v>
       </c>
       <c r="C53" s="7">
-        <f>(B53*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>871.24703160053332</v>
       </c>
       <c r="D53" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C53</f>
+        <f t="shared" si="8"/>
         <v>150.47117021396639</v>
       </c>
       <c r="E53" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F53" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>144055.93406021912</v>
       </c>
     </row>
@@ -8036,23 +8071,23 @@
         <v>44</v>
       </c>
       <c r="B54" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>144055.93406021912</v>
       </c>
       <c r="C54" s="7">
-        <f>(B54*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>870.33793494715712</v>
       </c>
       <c r="D54" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C54</f>
+        <f t="shared" si="8"/>
         <v>151.38026686734258</v>
       </c>
       <c r="E54" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F54" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>143904.55379335178</v>
       </c>
     </row>
@@ -8061,23 +8096,23 @@
         <v>45</v>
       </c>
       <c r="B55" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>143904.55379335178</v>
       </c>
       <c r="C55" s="7">
-        <f>(B55*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>869.42334583483364</v>
       </c>
       <c r="D55" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C55</f>
+        <f t="shared" si="8"/>
         <v>152.29485597966607</v>
       </c>
       <c r="E55" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F55" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>143752.2589373721</v>
       </c>
     </row>
@@ -8086,23 +8121,23 @@
         <v>46</v>
       </c>
       <c r="B56" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>143752.2589373721</v>
       </c>
       <c r="C56" s="7">
-        <f>(B56*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>868.50323107995644</v>
       </c>
       <c r="D56" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C56</f>
+        <f t="shared" si="8"/>
         <v>153.21497073454327</v>
       </c>
       <c r="E56" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F56" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>143599.04396663755</v>
       </c>
     </row>
@@ -8111,23 +8146,23 @@
         <v>47</v>
       </c>
       <c r="B57" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>143599.04396663755</v>
       </c>
       <c r="C57" s="7">
-        <f>(B57*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>867.57755729843518</v>
       </c>
       <c r="D57" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C57</f>
+        <f t="shared" si="8"/>
         <v>154.14064451606453</v>
       </c>
       <c r="E57" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F57" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>143444.90332212148</v>
       </c>
     </row>
@@ -8136,23 +8171,23 @@
         <v>48</v>
       </c>
       <c r="B58" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>143444.90332212148</v>
       </c>
       <c r="C58" s="7">
-        <f>(B58*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>866.64629090448386</v>
       </c>
       <c r="D58" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C58</f>
+        <f t="shared" si="8"/>
         <v>155.07191091001584</v>
       </c>
       <c r="E58" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F58" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>143289.83141121146</v>
       </c>
     </row>
@@ -8161,23 +8196,23 @@
         <v>49</v>
       </c>
       <c r="B59" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>143289.83141121146</v>
       </c>
       <c r="C59" s="7">
-        <f>(B59*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>865.70939810940251</v>
       </c>
       <c r="D59" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C59</f>
+        <f t="shared" si="8"/>
         <v>156.00880370509719</v>
       </c>
       <c r="E59" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F59" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>143133.82260750636</v>
       </c>
     </row>
@@ -8186,23 +8221,23 @@
         <v>50</v>
       </c>
       <c r="B60" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>143133.82260750636</v>
       </c>
       <c r="C60" s="7">
-        <f>(B60*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>864.76684492035088</v>
       </c>
       <c r="D60" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C60</f>
+        <f t="shared" si="8"/>
         <v>156.95135689414883</v>
       </c>
       <c r="E60" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F60" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142976.8712506122</v>
       </c>
     </row>
@@ -8211,23 +8246,23 @@
         <v>51</v>
       </c>
       <c r="B61" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>142976.8712506122</v>
       </c>
       <c r="C61" s="7">
-        <f>(B61*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>863.81859713911535</v>
       </c>
       <c r="D61" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C61</f>
+        <f t="shared" si="8"/>
         <v>157.89960467538435</v>
       </c>
       <c r="E61" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F61" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142818.97164593681</v>
       </c>
     </row>
@@ -8236,23 +8271,23 @@
         <v>52</v>
       </c>
       <c r="B62" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>142818.97164593681</v>
       </c>
       <c r="C62" s="7">
-        <f>(B62*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>862.86462036086823</v>
       </c>
       <c r="D62" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C62</f>
+        <f t="shared" si="8"/>
         <v>158.85358145363148</v>
       </c>
       <c r="E62" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F62" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142660.11806448316</v>
       </c>
     </row>
@@ -8261,23 +8296,23 @@
         <v>53</v>
       </c>
       <c r="B63" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>142660.11806448316</v>
       </c>
       <c r="C63" s="7">
-        <f>(B63*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>861.90487997291905</v>
       </c>
       <c r="D63" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C63</f>
+        <f t="shared" si="8"/>
         <v>159.81332184158066</v>
       </c>
       <c r="E63" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F63" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142500.30474264157</v>
       </c>
     </row>
@@ -8286,23 +8321,23 @@
         <v>54</v>
       </c>
       <c r="B64" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>142500.30474264157</v>
       </c>
       <c r="C64" s="7">
-        <f>(B64*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>860.93934115345951</v>
       </c>
       <c r="D64" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C64</f>
+        <f t="shared" si="8"/>
         <v>160.7788606610402</v>
       </c>
       <c r="E64" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F64" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142339.52588198055</v>
       </c>
     </row>
@@ -8311,23 +8346,23 @@
         <v>55</v>
       </c>
       <c r="B65" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>142339.52588198055</v>
       </c>
       <c r="C65" s="7">
-        <f>(B65*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>859.96796887029916</v>
       </c>
       <c r="D65" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C65</f>
+        <f t="shared" si="8"/>
         <v>161.75023294420055</v>
       </c>
       <c r="E65" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F65" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142177.77564903634</v>
       </c>
     </row>
@@ -8336,23 +8371,23 @@
         <v>56</v>
       </c>
       <c r="B66" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>142177.77564903634</v>
       </c>
       <c r="C66" s="7">
-        <f>(B66*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>858.99072787959449</v>
       </c>
       <c r="D66" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C66</f>
+        <f t="shared" si="8"/>
         <v>162.72747393490522</v>
       </c>
       <c r="E66" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F66" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142015.04817510143</v>
       </c>
     </row>
@@ -8361,23 +8396,23 @@
         <v>57</v>
       </c>
       <c r="B67" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>142015.04817510143</v>
       </c>
       <c r="C67" s="7">
-        <f>(B67*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>858.00758272457108</v>
       </c>
       <c r="D67" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C67</f>
+        <f t="shared" si="8"/>
         <v>163.71061908992863</v>
       </c>
       <c r="E67" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F67" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>141851.33755601151</v>
       </c>
     </row>
@@ -8386,23 +8421,23 @@
         <v>58</v>
       </c>
       <c r="B68" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>141851.33755601151</v>
       </c>
       <c r="C68" s="7">
-        <f>(B68*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>857.01849773423623</v>
       </c>
       <c r="D68" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C68</f>
+        <f t="shared" si="8"/>
         <v>164.69970408026347</v>
       </c>
       <c r="E68" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F68" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>141686.63785193124</v>
       </c>
     </row>
@@ -8411,23 +8446,23 @@
         <v>59</v>
       </c>
       <c r="B69" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>141686.63785193124</v>
       </c>
       <c r="C69" s="7">
-        <f>(B69*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>856.02343702208452</v>
       </c>
       <c r="D69" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C69</f>
+        <f t="shared" si="8"/>
         <v>165.69476479241519</v>
       </c>
       <c r="E69" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F69" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>141520.94308713882</v>
       </c>
     </row>
@@ -8436,23 +8471,23 @@
         <v>60</v>
       </c>
       <c r="B70" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>141520.94308713882</v>
       </c>
       <c r="C70" s="7">
-        <f>(B70*InterestRateAfterRateAdjust)</f>
+        <f t="shared" si="7"/>
         <v>855.02236448479698</v>
       </c>
       <c r="D70" s="7">
-        <f>MonthlyPaymentAfterRateAdjust-C70</f>
+        <f t="shared" si="8"/>
         <v>166.69583732970273</v>
       </c>
       <c r="E70" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F70" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>141354.24724980912</v>
       </c>
     </row>
@@ -8460,6 +8495,1609 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="3">
+        <f>B22</f>
+        <v>554.03435636993618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="C4" s="26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <f>B4/12</f>
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="C5" s="4">
+        <f>C4/12</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <f>-PMT(MonthlyInterestRate,NumPayments,LoanAmount,0,0)</f>
+        <v>43.871389734068444</v>
+      </c>
+      <c r="C7" s="1">
+        <f>-PMT(C5,C6,C3,0,0)</f>
+        <v>45.145333466778531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="3">
+        <f>LoanAmount</f>
+        <v>1000</v>
+      </c>
+      <c r="C11" s="3">
+        <f>(B11*B$5)</f>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ref="D11:D12" si="0">MonthlyPayment-C11</f>
+        <v>39.70472306740178</v>
+      </c>
+      <c r="E11" s="3">
+        <f>B$8</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <f>B11-SUM(D11:E11)</f>
+        <v>960.2952769325982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <f>F11</f>
+        <v>960.2952769325982</v>
+      </c>
+      <c r="C12" s="3">
+        <f>(B12*B$5)</f>
+        <v>4.0012303205524926</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>39.87015941351595</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ref="E12:E35" si="1">B$8</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" ref="F12" si="2">B12-SUM(D12:E12)</f>
+        <v>920.42511751908228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" ref="B13:B35" si="3">F12</f>
+        <v>920.42511751908228</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" ref="C13:C21" si="4">(B13*B$5)</f>
+        <v>3.8351046563295093</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" ref="D13:D21" si="5">MonthlyPayment-C13</f>
+        <v>40.036285077738938</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ref="F13:F35" si="6">B13-SUM(D13:E13)</f>
+        <v>880.38883244134331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="3"/>
+        <v>880.38883244134331</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="4"/>
+        <v>3.6682868018389305</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="5"/>
+        <v>40.203102932229513</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="6"/>
+        <v>840.1857295091138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="3"/>
+        <v>840.1857295091138</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="4"/>
+        <v>3.5007738729546407</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="5"/>
+        <v>40.370615861113805</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="6"/>
+        <v>799.81511364799996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="3"/>
+        <v>799.81511364799996</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="4"/>
+        <v>3.3325629735333333</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="5"/>
+        <v>40.538826760535109</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="6"/>
+        <v>759.27628688746483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="3"/>
+        <v>759.27628688746483</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="4"/>
+        <v>3.1636511953644368</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="5"/>
+        <v>40.707738538704007</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="6"/>
+        <v>718.56854834876083</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="3"/>
+        <v>718.56854834876083</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="4"/>
+        <v>2.9940356181198369</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="5"/>
+        <v>40.877354115948606</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="6"/>
+        <v>677.69119423281222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="3"/>
+        <v>677.69119423281222</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="4"/>
+        <v>2.8237133093033844</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="5"/>
+        <v>41.047676424765058</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="6"/>
+        <v>636.64351780804714</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="3"/>
+        <v>636.64351780804714</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="4"/>
+        <v>2.6526813242001963</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="5"/>
+        <v>41.218708409868249</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="6"/>
+        <v>595.42480939817892</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="3"/>
+        <v>595.42480939817892</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="4"/>
+        <v>2.4809367058257457</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="5"/>
+        <v>41.390453028242696</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="6"/>
+        <v>554.03435636993618</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="3"/>
+        <v>554.03435636993618</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" ref="C22:C35" si="7">(B22*InterestRateAfterRateAdjust)</f>
+        <v>4.6169529697494678</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" ref="D22:D35" si="8">MonthlyPaymentAfterRateAdjust-C22</f>
+        <v>40.528380497029062</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="6"/>
+        <v>513.50597587290713</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="3"/>
+        <v>513.50597587290713</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="7"/>
+        <v>4.2792164656075595</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="8"/>
+        <v>40.86611700117097</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="6"/>
+        <v>472.63985887173618</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>14</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="3"/>
+        <v>472.63985887173618</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="7"/>
+        <v>3.9386654905978014</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="8"/>
+        <v>41.206667976180732</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="6"/>
+        <v>431.43319089555547</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="3"/>
+        <v>431.43319089555547</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="7"/>
+        <v>3.5952765907962956</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="8"/>
+        <v>41.550056875982236</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="6"/>
+        <v>389.88313401957322</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="3"/>
+        <v>389.88313401957322</v>
+      </c>
+      <c r="C26" s="7">
+        <f t="shared" si="7"/>
+        <v>3.2490261168297767</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="8"/>
+        <v>41.896307349948756</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="6"/>
+        <v>347.98682666962446</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>17</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="3"/>
+        <v>347.98682666962446</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="7"/>
+        <v>2.8998902222468703</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="8"/>
+        <v>42.245443244531664</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="6"/>
+        <v>305.74138342509281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>18</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="3"/>
+        <v>305.74138342509281</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" si="7"/>
+        <v>2.5478448618757734</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="8"/>
+        <v>42.597488604902757</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="6"/>
+        <v>263.14389482019004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="3"/>
+        <v>263.14389482019004</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" si="7"/>
+        <v>2.1928657901682502</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="8"/>
+        <v>42.952467676610283</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="6"/>
+        <v>220.19142714357974</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="3"/>
+        <v>220.19142714357974</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="7"/>
+        <v>1.8349285595298312</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="8"/>
+        <v>43.310404907248703</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="6"/>
+        <v>176.88102223633103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="3"/>
+        <v>176.88102223633103</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="7"/>
+        <v>1.4740085186360918</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="8"/>
+        <v>43.671324948142441</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="6"/>
+        <v>133.20969728818858</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="3"/>
+        <v>133.20969728818858</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="7"/>
+        <v>1.1100808107349047</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="8"/>
+        <v>44.035252656043625</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="6"/>
+        <v>89.174444632144954</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="3"/>
+        <v>89.174444632144954</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="7"/>
+        <v>0.74312037193454128</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="8"/>
+        <v>44.402213094843987</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="6"/>
+        <v>44.772231537300968</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="3"/>
+        <v>44.772231537300968</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="7"/>
+        <v>0.37310192947750809</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="8"/>
+        <v>44.772231537301025</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="6"/>
+        <v>-5.6843418860808015E-14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>25</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="3"/>
+        <v>-5.6843418860808015E-14</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="7"/>
+        <v>-4.7369515717340012E-16</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="8"/>
+        <v>45.145333466778531</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="6"/>
+        <v>-45.145333466778588</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="1">
+        <f>D14</f>
+        <v>1012.5521556712963</v>
+      </c>
+      <c r="D3" s="3">
+        <f>B30</f>
+        <v>567.21288992933887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="C4" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D4" s="26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <f>B4/12</f>
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="C5" s="4">
+        <f>C4/12</f>
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="D5" s="4">
+        <f>D4/12</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <f>-PMT(MonthlyInterestRate,NumPayments,LoanAmount,0,0)</f>
+        <v>43.871389734068444</v>
+      </c>
+      <c r="C7" s="1">
+        <f>-PMT(C5,C6,C3,0,0)</f>
+        <v>45.564434543732652</v>
+      </c>
+      <c r="D7" s="1">
+        <f>-PMT(D5,D6,D3,0,0)</f>
+        <v>46.219182561698396</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="1">
+        <f>LoanAmount</f>
+        <v>1000</v>
+      </c>
+      <c r="C12" s="1">
+        <f>B12*B$5</f>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="D12" s="1">
+        <f>B12+C12</f>
+        <v>1004.1666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <f>D12</f>
+        <v>1004.1666666666666</v>
+      </c>
+      <c r="C13" s="1">
+        <f>B13*B$5</f>
+        <v>4.1840277777777777</v>
+      </c>
+      <c r="D13" s="1">
+        <f>B13+C13</f>
+        <v>1008.3506944444445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <f>D13</f>
+        <v>1008.3506944444445</v>
+      </c>
+      <c r="C14" s="1">
+        <f>B14*B$5</f>
+        <v>4.2014612268518521</v>
+      </c>
+      <c r="D14" s="1">
+        <f>B14+C14</f>
+        <v>1012.5521556712963</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="3">
+        <f>C3</f>
+        <v>1012.5521556712963</v>
+      </c>
+      <c r="C19" s="3">
+        <f>(B19*C$5)</f>
+        <v>6.3284509729456015</v>
+      </c>
+      <c r="D19" s="3">
+        <f>C$7-C19</f>
+        <v>39.235983570787049</v>
+      </c>
+      <c r="E19" s="3">
+        <f>B$8</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <f>B19-SUM(D19:E19)</f>
+        <v>973.31617210050922</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3">
+        <f>F19</f>
+        <v>973.31617210050922</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" ref="C20:C29" si="0">(B20*C$5)</f>
+        <v>6.0832260756281817</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" ref="D20:D29" si="1">C$7-C20</f>
+        <v>39.481208468104469</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" ref="E20:E43" si="2">B$8</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" ref="F20" si="3">B20-SUM(D20:E20)</f>
+        <v>933.83496363240477</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" ref="B21:B43" si="4">F20</f>
+        <v>933.83496363240477</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
+        <v>5.8364685227025292</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="1"/>
+        <v>39.72796602103012</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" ref="F21:F43" si="5">B21-SUM(D21:E21)</f>
+        <v>894.1069976113746</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="4"/>
+        <v>894.1069976113746</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="0"/>
+        <v>5.5881687350710907</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="1"/>
+        <v>39.976265808661559</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="5"/>
+        <v>854.13073180271306</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="4"/>
+        <v>854.13073180271306</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="0"/>
+        <v>5.3383170737669561</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="1"/>
+        <v>40.226117469965693</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="5"/>
+        <v>813.90461433274731</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3">
+        <f t="shared" si="4"/>
+        <v>813.90461433274731</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="0"/>
+        <v>5.0869038395796702</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="1"/>
+        <v>40.477530704152983</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="5"/>
+        <v>773.42708362859435</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3">
+        <f t="shared" si="4"/>
+        <v>773.42708362859435</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="0"/>
+        <v>4.8339192726787141</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="1"/>
+        <v>40.730515271053939</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="5"/>
+        <v>732.6965683575404</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3">
+        <f t="shared" si="4"/>
+        <v>732.6965683575404</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>4.5793535522346271</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="1"/>
+        <v>40.985080991498023</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="5"/>
+        <v>691.71148736604232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" s="3">
+        <f t="shared" si="4"/>
+        <v>691.71148736604232</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="0"/>
+        <v>4.323196796037764</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="1"/>
+        <v>41.241237747694889</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="5"/>
+        <v>650.47024961834745</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3">
+        <f t="shared" si="4"/>
+        <v>650.47024961834745</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="0"/>
+        <v>4.065439060114671</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="1"/>
+        <v>41.498995483617982</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="5"/>
+        <v>608.97125413472952</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>11</v>
+      </c>
+      <c r="B29" s="3">
+        <f t="shared" si="4"/>
+        <v>608.97125413472952</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8060703383420593</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="1"/>
+        <v>41.758364205390592</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="5"/>
+        <v>567.21288992933887</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="4"/>
+        <v>567.21288992933887</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" ref="C30:C43" si="6">(B30*InterestRateAfterRateAdjust)</f>
+        <v>4.7267740827444902</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" ref="D30:D43" si="7">MonthlyPaymentAfterRateAdjust-C30</f>
+        <v>41.492408478953905</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="5"/>
+        <v>525.72048145038502</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>13</v>
+      </c>
+      <c r="B31" s="3">
+        <f t="shared" si="4"/>
+        <v>525.72048145038502</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="6"/>
+        <v>4.3810040120865414</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="7"/>
+        <v>41.838178549611854</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="5"/>
+        <v>483.8823029007732</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>14</v>
+      </c>
+      <c r="B32" s="3">
+        <f t="shared" si="4"/>
+        <v>483.8823029007732</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="6"/>
+        <v>4.0323525241731097</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="7"/>
+        <v>42.186830037525283</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="5"/>
+        <v>441.69547286324791</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>15</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="4"/>
+        <v>441.69547286324791</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" si="6"/>
+        <v>3.6807956071937324</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="7"/>
+        <v>42.538386954504666</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="5"/>
+        <v>399.15708590874323</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>16</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="4"/>
+        <v>399.15708590874323</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="6"/>
+        <v>3.3263090492395269</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="7"/>
+        <v>42.89287351245887</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="5"/>
+        <v>356.26421239628434</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>17</v>
+      </c>
+      <c r="B35" s="3">
+        <f t="shared" si="4"/>
+        <v>356.26421239628434</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="6"/>
+        <v>2.9688684366357028</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="7"/>
+        <v>43.250314125062694</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="5"/>
+        <v>313.01389827122165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>18</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="4"/>
+        <v>313.01389827122165</v>
+      </c>
+      <c r="C36" s="7">
+        <f t="shared" si="6"/>
+        <v>2.6084491522601803</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="7"/>
+        <v>43.610733409438218</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="5"/>
+        <v>269.40316486178341</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>19</v>
+      </c>
+      <c r="B37" s="3">
+        <f t="shared" si="4"/>
+        <v>269.40316486178341</v>
+      </c>
+      <c r="C37" s="7">
+        <f t="shared" si="6"/>
+        <v>2.2450263738481953</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="7"/>
+        <v>43.974156187850198</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="5"/>
+        <v>225.4290086739332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>20</v>
+      </c>
+      <c r="B38" s="3">
+        <f t="shared" si="4"/>
+        <v>225.4290086739332</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" si="6"/>
+        <v>1.8785750722827765</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" si="7"/>
+        <v>44.340607489415618</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="5"/>
+        <v>181.08840118451758</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>21</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" si="4"/>
+        <v>181.08840118451758</v>
+      </c>
+      <c r="C39" s="7">
+        <f t="shared" si="6"/>
+        <v>1.5090700098709797</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="7"/>
+        <v>44.710112551827415</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="5"/>
+        <v>136.37828863269016</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>22</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="4"/>
+        <v>136.37828863269016</v>
+      </c>
+      <c r="C40" s="7">
+        <f t="shared" si="6"/>
+        <v>1.1364857386057512</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="7"/>
+        <v>45.082696823092647</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="5"/>
+        <v>91.295591809597511</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>23</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" si="4"/>
+        <v>91.295591809597511</v>
+      </c>
+      <c r="C41" s="7">
+        <f t="shared" si="6"/>
+        <v>0.7607965984133126</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="7"/>
+        <v>45.458385963285082</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="5"/>
+        <v>45.837205846312429</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" si="4"/>
+        <v>45.837205846312429</v>
+      </c>
+      <c r="C42" s="7">
+        <f t="shared" si="6"/>
+        <v>0.38197671538593692</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="7"/>
+        <v>45.837205846312457</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C43" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="7">
+        <f t="shared" si="7"/>
+        <v>46.219182561698396</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="5"/>
+        <v>-46.219182561698396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -10009,7 +11647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
@@ -12718,7 +14356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>